<commit_message>
Pit Fighter - 5 fights done, 2057 frames ahead
</commit_message>
<xml_diff>
--- a/PitFighter/PitFighter.xlsx
+++ b/PitFighter/PitFighter.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="213">
   <si>
     <t>Notes</t>
   </si>
@@ -696,18 +696,28 @@
   <si>
     <t>Start cartwheel</t>
   </si>
+  <si>
+    <t>Fight 6 begin</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="45">
+  <fonts count="46">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1586,34 +1596,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1621,185 +1631,185 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="25" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="26" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="25" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="25" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="26" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="26" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="36" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="27" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="25" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="28" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="26" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1809,10 +1819,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1824,7 +1834,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1833,128 +1843,131 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="43" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="44" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="44" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="33" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="43" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="35" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="34" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -2269,7 +2282,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="1"/>
@@ -2432,7 +2445,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A9" s="135"/>
+      <c r="A9" s="142"/>
       <c r="B9" s="98" t="s">
         <v>175</v>
       </c>
@@ -2442,8 +2455,8 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A10" s="135"/>
-      <c r="B10" s="197" t="s">
+      <c r="A10" s="142"/>
+      <c r="B10" s="135" t="s">
         <v>206</v>
       </c>
       <c r="C10" s="101">
@@ -2459,8 +2472,8 @@
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A11" s="135"/>
-      <c r="B11" s="197" t="s">
+      <c r="A11" s="142"/>
+      <c r="B11" s="135" t="s">
         <v>211</v>
       </c>
       <c r="C11" s="101">
@@ -2476,8 +2489,8 @@
       <c r="F11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A12" s="135"/>
-      <c r="B12" s="197" t="s">
+      <c r="A12" s="142"/>
+      <c r="B12" s="135" t="s">
         <v>208</v>
       </c>
       <c r="C12" s="101">
@@ -2493,8 +2506,8 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A13" s="135"/>
-      <c r="B13" s="197" t="s">
+      <c r="A13" s="142"/>
+      <c r="B13" s="135" t="s">
         <v>209</v>
       </c>
       <c r="C13" s="101"/>
@@ -2508,8 +2521,8 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A14" s="135"/>
-      <c r="B14" s="197" t="s">
+      <c r="A14" s="142"/>
+      <c r="B14" s="135" t="s">
         <v>210</v>
       </c>
       <c r="C14" s="101">
@@ -2525,15 +2538,24 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A15" s="135"/>
-      <c r="B15" s="100"/>
-      <c r="C15" s="101"/>
-      <c r="D15" s="101"/>
-      <c r="E15" s="101"/>
+      <c r="A15" s="142"/>
+      <c r="B15" s="198" t="s">
+        <v>212</v>
+      </c>
+      <c r="C15" s="101">
+        <v>5362</v>
+      </c>
+      <c r="D15" s="101">
+        <v>7419</v>
+      </c>
+      <c r="E15" s="101">
+        <f t="shared" si="0"/>
+        <v>2057</v>
+      </c>
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A16" s="135"/>
+      <c r="A16" s="142"/>
       <c r="B16" s="100"/>
       <c r="C16" s="101"/>
       <c r="D16" s="101"/>
@@ -2541,7 +2563,7 @@
       <c r="F16" s="105"/>
     </row>
     <row r="17" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A17" s="135"/>
+      <c r="A17" s="142"/>
       <c r="B17" s="100"/>
       <c r="C17" s="101"/>
       <c r="D17" s="101"/>
@@ -2552,7 +2574,7 @@
       <c r="F17" s="105"/>
     </row>
     <row r="18" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A18" s="135"/>
+      <c r="A18" s="142"/>
       <c r="B18" s="100"/>
       <c r="C18" s="101"/>
       <c r="D18" s="101"/>
@@ -2563,7 +2585,7 @@
       <c r="F18" s="105"/>
     </row>
     <row r="19" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A19" s="135"/>
+      <c r="A19" s="142"/>
       <c r="B19" s="100"/>
       <c r="C19" s="101"/>
       <c r="D19" s="101"/>
@@ -2574,7 +2596,7 @@
       <c r="F19" s="105"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A20" s="135"/>
+      <c r="A20" s="142"/>
       <c r="B20" s="98" t="s">
         <v>178</v>
       </c>
@@ -2653,13 +2675,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="161" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
+      <c r="B1" s="161"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -2689,18 +2711,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="143"/>
-      <c r="D3" s="144"/>
-      <c r="E3" s="144"/>
+      <c r="C3" s="162"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="145"/>
-      <c r="D4" s="146"/>
-      <c r="E4" s="146"/>
+      <c r="C4" s="143"/>
+      <c r="D4" s="144"/>
+      <c r="E4" s="144"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -2852,9 +2874,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="147"/>
-      <c r="D21" s="148"/>
-      <c r="E21" s="148"/>
+      <c r="C21" s="145"/>
+      <c r="D21" s="146"/>
+      <c r="E21" s="146"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -3005,9 +3027,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="145"/>
-      <c r="D38" s="146"/>
-      <c r="E38" s="146"/>
+      <c r="C38" s="143"/>
+      <c r="D38" s="144"/>
+      <c r="E38" s="144"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -3158,9 +3180,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="145"/>
-      <c r="D55" s="146"/>
-      <c r="E55" s="146"/>
+      <c r="C55" s="143"/>
+      <c r="D55" s="144"/>
+      <c r="E55" s="144"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -3311,9 +3333,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="145"/>
-      <c r="D72" s="146"/>
-      <c r="E72" s="146"/>
+      <c r="C72" s="143"/>
+      <c r="D72" s="144"/>
+      <c r="E72" s="144"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -3464,9 +3486,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="145"/>
-      <c r="D89" s="146"/>
-      <c r="E89" s="146"/>
+      <c r="C89" s="143"/>
+      <c r="D89" s="144"/>
+      <c r="E89" s="144"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -3617,9 +3639,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="145"/>
-      <c r="D106" s="146"/>
-      <c r="E106" s="146"/>
+      <c r="C106" s="143"/>
+      <c r="D106" s="144"/>
+      <c r="E106" s="144"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -3770,9 +3792,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="145"/>
-      <c r="D123" s="146"/>
-      <c r="E123" s="146"/>
+      <c r="C123" s="143"/>
+      <c r="D123" s="144"/>
+      <c r="E123" s="144"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -3923,9 +3945,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="145"/>
-      <c r="D140" s="146"/>
-      <c r="E140" s="146"/>
+      <c r="C140" s="143"/>
+      <c r="D140" s="144"/>
+      <c r="E140" s="144"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -4076,9 +4098,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="145"/>
-      <c r="D157" s="146"/>
-      <c r="E157" s="146"/>
+      <c r="C157" s="143"/>
+      <c r="D157" s="144"/>
+      <c r="E157" s="144"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -4229,9 +4251,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="145"/>
-      <c r="D174" s="146"/>
-      <c r="E174" s="146"/>
+      <c r="C174" s="143"/>
+      <c r="D174" s="144"/>
+      <c r="E174" s="144"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -4382,9 +4404,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="145"/>
-      <c r="D191" s="146"/>
-      <c r="E191" s="146"/>
+      <c r="C191" s="143"/>
+      <c r="D191" s="144"/>
+      <c r="E191" s="144"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -4535,9 +4557,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="145"/>
-      <c r="D208" s="146"/>
-      <c r="E208" s="146"/>
+      <c r="C208" s="143"/>
+      <c r="D208" s="144"/>
+      <c r="E208" s="144"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -4688,9 +4710,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="145"/>
-      <c r="D225" s="146"/>
-      <c r="E225" s="146"/>
+      <c r="C225" s="143"/>
+      <c r="D225" s="144"/>
+      <c r="E225" s="144"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -4841,9 +4863,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="145"/>
-      <c r="D242" s="146"/>
-      <c r="E242" s="146"/>
+      <c r="C242" s="143"/>
+      <c r="D242" s="144"/>
+      <c r="E242" s="144"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -4994,9 +5016,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="145"/>
-      <c r="D259" s="146"/>
-      <c r="E259" s="146"/>
+      <c r="C259" s="143"/>
+      <c r="D259" s="144"/>
+      <c r="E259" s="144"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -5147,18 +5169,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="149"/>
-      <c r="D276" s="150"/>
-      <c r="E276" s="150"/>
+      <c r="C276" s="159"/>
+      <c r="D276" s="160"/>
+      <c r="E276" s="160"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="145"/>
-      <c r="D277" s="146"/>
-      <c r="E277" s="146"/>
+      <c r="C277" s="143"/>
+      <c r="D277" s="144"/>
+      <c r="E277" s="144"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -5309,9 +5331,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="147"/>
-      <c r="D294" s="148"/>
-      <c r="E294" s="148"/>
+      <c r="C294" s="145"/>
+      <c r="D294" s="146"/>
+      <c r="E294" s="146"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -5462,9 +5484,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="145"/>
-      <c r="D311" s="146"/>
-      <c r="E311" s="146"/>
+      <c r="C311" s="143"/>
+      <c r="D311" s="144"/>
+      <c r="E311" s="144"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -5615,9 +5637,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="145"/>
-      <c r="D328" s="146"/>
-      <c r="E328" s="146"/>
+      <c r="C328" s="143"/>
+      <c r="D328" s="144"/>
+      <c r="E328" s="144"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -5768,9 +5790,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="145"/>
-      <c r="D345" s="146"/>
-      <c r="E345" s="146"/>
+      <c r="C345" s="143"/>
+      <c r="D345" s="144"/>
+      <c r="E345" s="144"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -5921,9 +5943,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="145"/>
-      <c r="D362" s="146"/>
-      <c r="E362" s="146"/>
+      <c r="C362" s="143"/>
+      <c r="D362" s="144"/>
+      <c r="E362" s="144"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -6074,9 +6096,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="145"/>
-      <c r="D379" s="146"/>
-      <c r="E379" s="146"/>
+      <c r="C379" s="143"/>
+      <c r="D379" s="144"/>
+      <c r="E379" s="144"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -6227,9 +6249,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="145"/>
-      <c r="D396" s="146"/>
-      <c r="E396" s="146"/>
+      <c r="C396" s="143"/>
+      <c r="D396" s="144"/>
+      <c r="E396" s="144"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -6380,9 +6402,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="145"/>
-      <c r="D413" s="146"/>
-      <c r="E413" s="146"/>
+      <c r="C413" s="143"/>
+      <c r="D413" s="144"/>
+      <c r="E413" s="144"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -6533,9 +6555,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="145"/>
-      <c r="D430" s="146"/>
-      <c r="E430" s="146"/>
+      <c r="C430" s="143"/>
+      <c r="D430" s="144"/>
+      <c r="E430" s="144"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -6686,9 +6708,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="145"/>
-      <c r="D447" s="146"/>
-      <c r="E447" s="146"/>
+      <c r="C447" s="143"/>
+      <c r="D447" s="144"/>
+      <c r="E447" s="144"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -6839,9 +6861,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="145"/>
-      <c r="D464" s="146"/>
-      <c r="E464" s="146"/>
+      <c r="C464" s="143"/>
+      <c r="D464" s="144"/>
+      <c r="E464" s="144"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -6992,9 +7014,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="145"/>
-      <c r="D481" s="146"/>
-      <c r="E481" s="146"/>
+      <c r="C481" s="143"/>
+      <c r="D481" s="144"/>
+      <c r="E481" s="144"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -7145,9 +7167,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="145"/>
-      <c r="D498" s="146"/>
-      <c r="E498" s="146"/>
+      <c r="C498" s="143"/>
+      <c r="D498" s="144"/>
+      <c r="E498" s="144"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -7298,9 +7320,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="145"/>
-      <c r="D515" s="146"/>
-      <c r="E515" s="146"/>
+      <c r="C515" s="143"/>
+      <c r="D515" s="144"/>
+      <c r="E515" s="144"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -7451,9 +7473,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="145"/>
-      <c r="D532" s="146"/>
-      <c r="E532" s="146"/>
+      <c r="C532" s="143"/>
+      <c r="D532" s="144"/>
+      <c r="E532" s="144"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -7604,18 +7626,18 @@
         <v>49</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="151"/>
-      <c r="D549" s="152"/>
-      <c r="E549" s="152"/>
+      <c r="C549" s="157"/>
+      <c r="D549" s="158"/>
+      <c r="E549" s="158"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>50</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="145"/>
-      <c r="D550" s="146"/>
-      <c r="E550" s="146"/>
+      <c r="C550" s="143"/>
+      <c r="D550" s="144"/>
+      <c r="E550" s="144"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -7766,9 +7788,9 @@
         <v>51</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="147"/>
-      <c r="D567" s="148"/>
-      <c r="E567" s="148"/>
+      <c r="C567" s="145"/>
+      <c r="D567" s="146"/>
+      <c r="E567" s="146"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -7919,9 +7941,9 @@
         <v>52</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="145"/>
-      <c r="D584" s="146"/>
-      <c r="E584" s="146"/>
+      <c r="C584" s="143"/>
+      <c r="D584" s="144"/>
+      <c r="E584" s="144"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -8072,9 +8094,9 @@
         <v>53</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="145"/>
-      <c r="D601" s="146"/>
-      <c r="E601" s="146"/>
+      <c r="C601" s="143"/>
+      <c r="D601" s="144"/>
+      <c r="E601" s="144"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -8225,9 +8247,9 @@
         <v>54</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="145"/>
-      <c r="D618" s="146"/>
-      <c r="E618" s="146"/>
+      <c r="C618" s="143"/>
+      <c r="D618" s="144"/>
+      <c r="E618" s="144"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -8378,9 +8400,9 @@
         <v>55</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="145"/>
-      <c r="D635" s="146"/>
-      <c r="E635" s="146"/>
+      <c r="C635" s="143"/>
+      <c r="D635" s="144"/>
+      <c r="E635" s="144"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -8531,9 +8553,9 @@
         <v>56</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="145"/>
-      <c r="D652" s="146"/>
-      <c r="E652" s="146"/>
+      <c r="C652" s="143"/>
+      <c r="D652" s="144"/>
+      <c r="E652" s="144"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -8684,9 +8706,9 @@
         <v>57</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="145"/>
-      <c r="D669" s="146"/>
-      <c r="E669" s="146"/>
+      <c r="C669" s="143"/>
+      <c r="D669" s="144"/>
+      <c r="E669" s="144"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -8837,9 +8859,9 @@
         <v>58</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="145"/>
-      <c r="D686" s="146"/>
-      <c r="E686" s="146"/>
+      <c r="C686" s="143"/>
+      <c r="D686" s="144"/>
+      <c r="E686" s="144"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -8990,9 +9012,9 @@
         <v>59</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="145"/>
-      <c r="D703" s="146"/>
-      <c r="E703" s="146"/>
+      <c r="C703" s="143"/>
+      <c r="D703" s="144"/>
+      <c r="E703" s="144"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -9143,9 +9165,9 @@
         <v>60</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="145"/>
-      <c r="D720" s="146"/>
-      <c r="E720" s="146"/>
+      <c r="C720" s="143"/>
+      <c r="D720" s="144"/>
+      <c r="E720" s="144"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -9296,9 +9318,9 @@
         <v>61</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="145"/>
-      <c r="D737" s="146"/>
-      <c r="E737" s="146"/>
+      <c r="C737" s="143"/>
+      <c r="D737" s="144"/>
+      <c r="E737" s="144"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -9449,9 +9471,9 @@
         <v>62</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="145"/>
-      <c r="D754" s="146"/>
-      <c r="E754" s="146"/>
+      <c r="C754" s="143"/>
+      <c r="D754" s="144"/>
+      <c r="E754" s="144"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -9602,9 +9624,9 @@
         <v>63</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="145"/>
-      <c r="D771" s="146"/>
-      <c r="E771" s="146"/>
+      <c r="C771" s="143"/>
+      <c r="D771" s="144"/>
+      <c r="E771" s="144"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -9755,9 +9777,9 @@
         <v>64</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="145"/>
-      <c r="D788" s="146"/>
-      <c r="E788" s="146"/>
+      <c r="C788" s="143"/>
+      <c r="D788" s="144"/>
+      <c r="E788" s="144"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -9908,9 +9930,9 @@
         <v>65</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="145"/>
-      <c r="D805" s="146"/>
-      <c r="E805" s="146"/>
+      <c r="C805" s="143"/>
+      <c r="D805" s="144"/>
+      <c r="E805" s="144"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -10061,18 +10083,18 @@
         <v>66</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="153"/>
-      <c r="D822" s="154"/>
-      <c r="E822" s="154"/>
+      <c r="C822" s="155"/>
+      <c r="D822" s="156"/>
+      <c r="E822" s="156"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>67</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="145"/>
-      <c r="D823" s="146"/>
-      <c r="E823" s="146"/>
+      <c r="C823" s="143"/>
+      <c r="D823" s="144"/>
+      <c r="E823" s="144"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -10223,9 +10245,9 @@
         <v>68</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="147"/>
-      <c r="D840" s="148"/>
-      <c r="E840" s="148"/>
+      <c r="C840" s="145"/>
+      <c r="D840" s="146"/>
+      <c r="E840" s="146"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -10376,9 +10398,9 @@
         <v>69</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="145"/>
-      <c r="D857" s="146"/>
-      <c r="E857" s="146"/>
+      <c r="C857" s="143"/>
+      <c r="D857" s="144"/>
+      <c r="E857" s="144"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -10529,9 +10551,9 @@
         <v>70</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="145"/>
-      <c r="D874" s="146"/>
-      <c r="E874" s="146"/>
+      <c r="C874" s="143"/>
+      <c r="D874" s="144"/>
+      <c r="E874" s="144"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -10682,9 +10704,9 @@
         <v>71</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="145"/>
-      <c r="D891" s="146"/>
-      <c r="E891" s="146"/>
+      <c r="C891" s="143"/>
+      <c r="D891" s="144"/>
+      <c r="E891" s="144"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -10835,9 +10857,9 @@
         <v>72</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="145"/>
-      <c r="D908" s="146"/>
-      <c r="E908" s="146"/>
+      <c r="C908" s="143"/>
+      <c r="D908" s="144"/>
+      <c r="E908" s="144"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -10988,9 +11010,9 @@
         <v>73</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="145"/>
-      <c r="D925" s="146"/>
-      <c r="E925" s="146"/>
+      <c r="C925" s="143"/>
+      <c r="D925" s="144"/>
+      <c r="E925" s="144"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -11141,9 +11163,9 @@
         <v>74</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="145"/>
-      <c r="D942" s="146"/>
-      <c r="E942" s="146"/>
+      <c r="C942" s="143"/>
+      <c r="D942" s="144"/>
+      <c r="E942" s="144"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -11294,9 +11316,9 @@
         <v>75</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="145"/>
-      <c r="D959" s="146"/>
-      <c r="E959" s="146"/>
+      <c r="C959" s="143"/>
+      <c r="D959" s="144"/>
+      <c r="E959" s="144"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -11447,9 +11469,9 @@
         <v>76</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="145"/>
-      <c r="D976" s="146"/>
-      <c r="E976" s="146"/>
+      <c r="C976" s="143"/>
+      <c r="D976" s="144"/>
+      <c r="E976" s="144"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -11600,9 +11622,9 @@
         <v>77</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="145"/>
-      <c r="D993" s="146"/>
-      <c r="E993" s="146"/>
+      <c r="C993" s="143"/>
+      <c r="D993" s="144"/>
+      <c r="E993" s="144"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -11753,9 +11775,9 @@
         <v>78</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="145"/>
-      <c r="D1010" s="146"/>
-      <c r="E1010" s="146"/>
+      <c r="C1010" s="143"/>
+      <c r="D1010" s="144"/>
+      <c r="E1010" s="144"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -11906,9 +11928,9 @@
         <v>79</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="145"/>
-      <c r="D1027" s="146"/>
-      <c r="E1027" s="146"/>
+      <c r="C1027" s="143"/>
+      <c r="D1027" s="144"/>
+      <c r="E1027" s="144"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -12059,9 +12081,9 @@
         <v>82</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="145"/>
-      <c r="D1044" s="146"/>
-      <c r="E1044" s="146"/>
+      <c r="C1044" s="143"/>
+      <c r="D1044" s="144"/>
+      <c r="E1044" s="144"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -12212,9 +12234,9 @@
         <v>81</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="145"/>
-      <c r="D1061" s="146"/>
-      <c r="E1061" s="146"/>
+      <c r="C1061" s="143"/>
+      <c r="D1061" s="144"/>
+      <c r="E1061" s="144"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -12365,9 +12387,9 @@
         <v>83</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="145"/>
-      <c r="D1078" s="146"/>
-      <c r="E1078" s="146"/>
+      <c r="C1078" s="143"/>
+      <c r="D1078" s="144"/>
+      <c r="E1078" s="144"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -12518,18 +12540,18 @@
         <v>103</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="155"/>
-      <c r="D1095" s="156"/>
-      <c r="E1095" s="156"/>
+      <c r="C1095" s="153"/>
+      <c r="D1095" s="154"/>
+      <c r="E1095" s="154"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>84</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="145"/>
-      <c r="D1096" s="146"/>
-      <c r="E1096" s="146"/>
+      <c r="C1096" s="143"/>
+      <c r="D1096" s="144"/>
+      <c r="E1096" s="144"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -12680,9 +12702,9 @@
         <v>85</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="147"/>
-      <c r="D1113" s="148"/>
-      <c r="E1113" s="148"/>
+      <c r="C1113" s="145"/>
+      <c r="D1113" s="146"/>
+      <c r="E1113" s="146"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -12833,9 +12855,9 @@
         <v>86</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="145"/>
-      <c r="D1130" s="146"/>
-      <c r="E1130" s="146"/>
+      <c r="C1130" s="143"/>
+      <c r="D1130" s="144"/>
+      <c r="E1130" s="144"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -12986,9 +13008,9 @@
         <v>87</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="145"/>
-      <c r="D1147" s="146"/>
-      <c r="E1147" s="146"/>
+      <c r="C1147" s="143"/>
+      <c r="D1147" s="144"/>
+      <c r="E1147" s="144"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -13139,9 +13161,9 @@
         <v>88</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="145"/>
-      <c r="D1164" s="146"/>
-      <c r="E1164" s="146"/>
+      <c r="C1164" s="143"/>
+      <c r="D1164" s="144"/>
+      <c r="E1164" s="144"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -13292,9 +13314,9 @@
         <v>89</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="145"/>
-      <c r="D1181" s="146"/>
-      <c r="E1181" s="146"/>
+      <c r="C1181" s="143"/>
+      <c r="D1181" s="144"/>
+      <c r="E1181" s="144"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -13445,9 +13467,9 @@
         <v>90</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="145"/>
-      <c r="D1198" s="146"/>
-      <c r="E1198" s="146"/>
+      <c r="C1198" s="143"/>
+      <c r="D1198" s="144"/>
+      <c r="E1198" s="144"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -13598,9 +13620,9 @@
         <v>91</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="145"/>
-      <c r="D1215" s="146"/>
-      <c r="E1215" s="146"/>
+      <c r="C1215" s="143"/>
+      <c r="D1215" s="144"/>
+      <c r="E1215" s="144"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -13751,9 +13773,9 @@
         <v>92</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="145"/>
-      <c r="D1232" s="146"/>
-      <c r="E1232" s="146"/>
+      <c r="C1232" s="143"/>
+      <c r="D1232" s="144"/>
+      <c r="E1232" s="144"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -13904,9 +13926,9 @@
         <v>93</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="145"/>
-      <c r="D1249" s="146"/>
-      <c r="E1249" s="146"/>
+      <c r="C1249" s="143"/>
+      <c r="D1249" s="144"/>
+      <c r="E1249" s="144"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -14057,9 +14079,9 @@
         <v>98</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="145"/>
-      <c r="D1266" s="146"/>
-      <c r="E1266" s="146"/>
+      <c r="C1266" s="143"/>
+      <c r="D1266" s="144"/>
+      <c r="E1266" s="144"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -14210,9 +14232,9 @@
         <v>99</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="145"/>
-      <c r="D1283" s="146"/>
-      <c r="E1283" s="146"/>
+      <c r="C1283" s="143"/>
+      <c r="D1283" s="144"/>
+      <c r="E1283" s="144"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -14363,9 +14385,9 @@
         <v>100</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="145"/>
-      <c r="D1300" s="146"/>
-      <c r="E1300" s="146"/>
+      <c r="C1300" s="143"/>
+      <c r="D1300" s="144"/>
+      <c r="E1300" s="144"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -14516,9 +14538,9 @@
         <v>80</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="145"/>
-      <c r="D1317" s="146"/>
-      <c r="E1317" s="146"/>
+      <c r="C1317" s="143"/>
+      <c r="D1317" s="144"/>
+      <c r="E1317" s="144"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -14669,9 +14691,9 @@
         <v>101</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="145"/>
-      <c r="D1334" s="146"/>
-      <c r="E1334" s="146"/>
+      <c r="C1334" s="143"/>
+      <c r="D1334" s="144"/>
+      <c r="E1334" s="144"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -14822,9 +14844,9 @@
         <v>97</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="145"/>
-      <c r="D1351" s="146"/>
-      <c r="E1351" s="146"/>
+      <c r="C1351" s="143"/>
+      <c r="D1351" s="144"/>
+      <c r="E1351" s="144"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -14975,18 +14997,18 @@
         <v>102</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="157"/>
-      <c r="D1368" s="158"/>
-      <c r="E1368" s="158"/>
+      <c r="C1368" s="151"/>
+      <c r="D1368" s="152"/>
+      <c r="E1368" s="152"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>104</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="145"/>
-      <c r="D1369" s="146"/>
-      <c r="E1369" s="146"/>
+      <c r="C1369" s="143"/>
+      <c r="D1369" s="144"/>
+      <c r="E1369" s="144"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -15137,9 +15159,9 @@
         <v>105</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="147"/>
-      <c r="D1386" s="148"/>
-      <c r="E1386" s="148"/>
+      <c r="C1386" s="145"/>
+      <c r="D1386" s="146"/>
+      <c r="E1386" s="146"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -15290,9 +15312,9 @@
         <v>106</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="145"/>
-      <c r="D1403" s="146"/>
-      <c r="E1403" s="146"/>
+      <c r="C1403" s="143"/>
+      <c r="D1403" s="144"/>
+      <c r="E1403" s="144"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -15443,9 +15465,9 @@
         <v>107</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="145"/>
-      <c r="D1420" s="146"/>
-      <c r="E1420" s="146"/>
+      <c r="C1420" s="143"/>
+      <c r="D1420" s="144"/>
+      <c r="E1420" s="144"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -15596,9 +15618,9 @@
         <v>108</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="145"/>
-      <c r="D1437" s="146"/>
-      <c r="E1437" s="146"/>
+      <c r="C1437" s="143"/>
+      <c r="D1437" s="144"/>
+      <c r="E1437" s="144"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -15749,9 +15771,9 @@
         <v>109</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="145"/>
-      <c r="D1454" s="146"/>
-      <c r="E1454" s="146"/>
+      <c r="C1454" s="143"/>
+      <c r="D1454" s="144"/>
+      <c r="E1454" s="144"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -15902,9 +15924,9 @@
         <v>110</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="145"/>
-      <c r="D1471" s="146"/>
-      <c r="E1471" s="146"/>
+      <c r="C1471" s="143"/>
+      <c r="D1471" s="144"/>
+      <c r="E1471" s="144"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -16055,9 +16077,9 @@
         <v>111</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="145"/>
-      <c r="D1488" s="146"/>
-      <c r="E1488" s="146"/>
+      <c r="C1488" s="143"/>
+      <c r="D1488" s="144"/>
+      <c r="E1488" s="144"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -16208,9 +16230,9 @@
         <v>112</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="145"/>
-      <c r="D1505" s="146"/>
-      <c r="E1505" s="146"/>
+      <c r="C1505" s="143"/>
+      <c r="D1505" s="144"/>
+      <c r="E1505" s="144"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -16361,9 +16383,9 @@
         <v>113</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="145"/>
-      <c r="D1522" s="146"/>
-      <c r="E1522" s="146"/>
+      <c r="C1522" s="143"/>
+      <c r="D1522" s="144"/>
+      <c r="E1522" s="144"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -16514,9 +16536,9 @@
         <v>94</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="145"/>
-      <c r="D1539" s="146"/>
-      <c r="E1539" s="146"/>
+      <c r="C1539" s="143"/>
+      <c r="D1539" s="144"/>
+      <c r="E1539" s="144"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -16667,9 +16689,9 @@
         <v>114</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="145"/>
-      <c r="D1556" s="146"/>
-      <c r="E1556" s="146"/>
+      <c r="C1556" s="143"/>
+      <c r="D1556" s="144"/>
+      <c r="E1556" s="144"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -16820,9 +16842,9 @@
         <v>115</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="145"/>
-      <c r="D1573" s="146"/>
-      <c r="E1573" s="146"/>
+      <c r="C1573" s="143"/>
+      <c r="D1573" s="144"/>
+      <c r="E1573" s="144"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -16973,9 +16995,9 @@
         <v>116</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="145"/>
-      <c r="D1590" s="146"/>
-      <c r="E1590" s="146"/>
+      <c r="C1590" s="143"/>
+      <c r="D1590" s="144"/>
+      <c r="E1590" s="144"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -17126,9 +17148,9 @@
         <v>117</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="145"/>
-      <c r="D1607" s="146"/>
-      <c r="E1607" s="146"/>
+      <c r="C1607" s="143"/>
+      <c r="D1607" s="144"/>
+      <c r="E1607" s="144"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -17279,9 +17301,9 @@
         <v>118</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="145"/>
-      <c r="D1624" s="146"/>
-      <c r="E1624" s="146"/>
+      <c r="C1624" s="143"/>
+      <c r="D1624" s="144"/>
+      <c r="E1624" s="144"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -17432,18 +17454,18 @@
         <v>119</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="159"/>
-      <c r="D1641" s="160"/>
-      <c r="E1641" s="160"/>
+      <c r="C1641" s="149"/>
+      <c r="D1641" s="150"/>
+      <c r="E1641" s="150"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>120</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="145"/>
-      <c r="D1642" s="146"/>
-      <c r="E1642" s="146"/>
+      <c r="C1642" s="143"/>
+      <c r="D1642" s="144"/>
+      <c r="E1642" s="144"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -17594,9 +17616,9 @@
         <v>121</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="147"/>
-      <c r="D1659" s="148"/>
-      <c r="E1659" s="148"/>
+      <c r="C1659" s="145"/>
+      <c r="D1659" s="146"/>
+      <c r="E1659" s="146"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -17747,9 +17769,9 @@
         <v>122</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="145"/>
-      <c r="D1676" s="146"/>
-      <c r="E1676" s="146"/>
+      <c r="C1676" s="143"/>
+      <c r="D1676" s="144"/>
+      <c r="E1676" s="144"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -17900,9 +17922,9 @@
         <v>123</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="145"/>
-      <c r="D1693" s="146"/>
-      <c r="E1693" s="146"/>
+      <c r="C1693" s="143"/>
+      <c r="D1693" s="144"/>
+      <c r="E1693" s="144"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -18053,9 +18075,9 @@
         <v>124</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="145"/>
-      <c r="D1710" s="146"/>
-      <c r="E1710" s="146"/>
+      <c r="C1710" s="143"/>
+      <c r="D1710" s="144"/>
+      <c r="E1710" s="144"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -18206,9 +18228,9 @@
         <v>125</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="145"/>
-      <c r="D1727" s="146"/>
-      <c r="E1727" s="146"/>
+      <c r="C1727" s="143"/>
+      <c r="D1727" s="144"/>
+      <c r="E1727" s="144"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -18359,9 +18381,9 @@
         <v>126</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="145"/>
-      <c r="D1744" s="146"/>
-      <c r="E1744" s="146"/>
+      <c r="C1744" s="143"/>
+      <c r="D1744" s="144"/>
+      <c r="E1744" s="144"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -18512,9 +18534,9 @@
         <v>127</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="145"/>
-      <c r="D1761" s="146"/>
-      <c r="E1761" s="146"/>
+      <c r="C1761" s="143"/>
+      <c r="D1761" s="144"/>
+      <c r="E1761" s="144"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -18665,9 +18687,9 @@
         <v>128</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="145"/>
-      <c r="D1778" s="146"/>
-      <c r="E1778" s="146"/>
+      <c r="C1778" s="143"/>
+      <c r="D1778" s="144"/>
+      <c r="E1778" s="144"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -18818,9 +18840,9 @@
         <v>129</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="145"/>
-      <c r="D1795" s="146"/>
-      <c r="E1795" s="146"/>
+      <c r="C1795" s="143"/>
+      <c r="D1795" s="144"/>
+      <c r="E1795" s="144"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -18971,9 +18993,9 @@
         <v>130</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="145"/>
-      <c r="D1812" s="146"/>
-      <c r="E1812" s="146"/>
+      <c r="C1812" s="143"/>
+      <c r="D1812" s="144"/>
+      <c r="E1812" s="144"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -19124,9 +19146,9 @@
         <v>95</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="145"/>
-      <c r="D1829" s="146"/>
-      <c r="E1829" s="146"/>
+      <c r="C1829" s="143"/>
+      <c r="D1829" s="144"/>
+      <c r="E1829" s="144"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -19277,9 +19299,9 @@
         <v>131</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="145"/>
-      <c r="D1846" s="146"/>
-      <c r="E1846" s="146"/>
+      <c r="C1846" s="143"/>
+      <c r="D1846" s="144"/>
+      <c r="E1846" s="144"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -19430,9 +19452,9 @@
         <v>132</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="145"/>
-      <c r="D1863" s="146"/>
-      <c r="E1863" s="146"/>
+      <c r="C1863" s="143"/>
+      <c r="D1863" s="144"/>
+      <c r="E1863" s="144"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -19583,9 +19605,9 @@
         <v>133</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="145"/>
-      <c r="D1880" s="146"/>
-      <c r="E1880" s="146"/>
+      <c r="C1880" s="143"/>
+      <c r="D1880" s="144"/>
+      <c r="E1880" s="144"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -19736,9 +19758,9 @@
         <v>134</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="145"/>
-      <c r="D1897" s="146"/>
-      <c r="E1897" s="146"/>
+      <c r="C1897" s="143"/>
+      <c r="D1897" s="144"/>
+      <c r="E1897" s="144"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -19889,18 +19911,18 @@
         <v>135</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="161"/>
-      <c r="D1914" s="162"/>
-      <c r="E1914" s="162"/>
+      <c r="C1914" s="147"/>
+      <c r="D1914" s="148"/>
+      <c r="E1914" s="148"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>136</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="145"/>
-      <c r="D1915" s="146"/>
-      <c r="E1915" s="146"/>
+      <c r="C1915" s="143"/>
+      <c r="D1915" s="144"/>
+      <c r="E1915" s="144"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -20051,9 +20073,9 @@
         <v>137</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="147"/>
-      <c r="D1932" s="148"/>
-      <c r="E1932" s="148"/>
+      <c r="C1932" s="145"/>
+      <c r="D1932" s="146"/>
+      <c r="E1932" s="146"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -20204,9 +20226,9 @@
         <v>138</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="145"/>
-      <c r="D1949" s="146"/>
-      <c r="E1949" s="146"/>
+      <c r="C1949" s="143"/>
+      <c r="D1949" s="144"/>
+      <c r="E1949" s="144"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -20357,9 +20379,9 @@
         <v>139</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="145"/>
-      <c r="D1966" s="146"/>
-      <c r="E1966" s="146"/>
+      <c r="C1966" s="143"/>
+      <c r="D1966" s="144"/>
+      <c r="E1966" s="144"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -20510,9 +20532,9 @@
         <v>140</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="145"/>
-      <c r="D1983" s="146"/>
-      <c r="E1983" s="146"/>
+      <c r="C1983" s="143"/>
+      <c r="D1983" s="144"/>
+      <c r="E1983" s="144"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -20663,9 +20685,9 @@
         <v>141</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="145"/>
-      <c r="D2000" s="146"/>
-      <c r="E2000" s="146"/>
+      <c r="C2000" s="143"/>
+      <c r="D2000" s="144"/>
+      <c r="E2000" s="144"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -20816,9 +20838,9 @@
         <v>142</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="145"/>
-      <c r="D2017" s="146"/>
-      <c r="E2017" s="146"/>
+      <c r="C2017" s="143"/>
+      <c r="D2017" s="144"/>
+      <c r="E2017" s="144"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -20969,9 +20991,9 @@
         <v>143</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="145"/>
-      <c r="D2034" s="146"/>
-      <c r="E2034" s="146"/>
+      <c r="C2034" s="143"/>
+      <c r="D2034" s="144"/>
+      <c r="E2034" s="144"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -21122,9 +21144,9 @@
         <v>144</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="145"/>
-      <c r="D2051" s="146"/>
-      <c r="E2051" s="146"/>
+      <c r="C2051" s="143"/>
+      <c r="D2051" s="144"/>
+      <c r="E2051" s="144"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -21275,9 +21297,9 @@
         <v>145</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="145"/>
-      <c r="D2068" s="146"/>
-      <c r="E2068" s="146"/>
+      <c r="C2068" s="143"/>
+      <c r="D2068" s="144"/>
+      <c r="E2068" s="144"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -21428,9 +21450,9 @@
         <v>146</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="145"/>
-      <c r="D2085" s="146"/>
-      <c r="E2085" s="146"/>
+      <c r="C2085" s="143"/>
+      <c r="D2085" s="144"/>
+      <c r="E2085" s="144"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -21581,9 +21603,9 @@
         <v>147</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="145"/>
-      <c r="D2102" s="146"/>
-      <c r="E2102" s="146"/>
+      <c r="C2102" s="143"/>
+      <c r="D2102" s="144"/>
+      <c r="E2102" s="144"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -21734,9 +21756,9 @@
         <v>96</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="145"/>
-      <c r="D2119" s="146"/>
-      <c r="E2119" s="146"/>
+      <c r="C2119" s="143"/>
+      <c r="D2119" s="144"/>
+      <c r="E2119" s="144"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -21887,9 +21909,9 @@
         <v>148</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="145"/>
-      <c r="D2136" s="146"/>
-      <c r="E2136" s="146"/>
+      <c r="C2136" s="143"/>
+      <c r="D2136" s="144"/>
+      <c r="E2136" s="144"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -22040,9 +22062,9 @@
         <v>149</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="145"/>
-      <c r="D2153" s="146"/>
-      <c r="E2153" s="146"/>
+      <c r="C2153" s="143"/>
+      <c r="D2153" s="144"/>
+      <c r="E2153" s="144"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -22193,9 +22215,9 @@
         <v>150</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="145"/>
-      <c r="D2170" s="146"/>
-      <c r="E2170" s="146"/>
+      <c r="C2170" s="143"/>
+      <c r="D2170" s="144"/>
+      <c r="E2170" s="144"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -22343,15 +22365,122 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
     <mergeCell ref="C1932:E1932"/>
     <mergeCell ref="C1949:E1949"/>
     <mergeCell ref="C1966:E1966"/>
@@ -22364,124 +22493,17 @@
     <mergeCell ref="C1897:E1897"/>
     <mergeCell ref="C1914:E1914"/>
     <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -22506,51 +22528,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="170" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="169"/>
-      <c r="C1" s="169"/>
-      <c r="D1" s="169"/>
-      <c r="E1" s="169"/>
-      <c r="F1" s="169"/>
-      <c r="G1" s="169"/>
-      <c r="H1" s="169"/>
-      <c r="I1" s="169"/>
-      <c r="J1" s="169"/>
-      <c r="K1" s="169"/>
-      <c r="L1" s="169"/>
+      <c r="B1" s="170"/>
+      <c r="C1" s="170"/>
+      <c r="D1" s="170"/>
+      <c r="E1" s="170"/>
+      <c r="F1" s="170"/>
+      <c r="G1" s="170"/>
+      <c r="H1" s="170"/>
+      <c r="I1" s="170"/>
+      <c r="J1" s="170"/>
+      <c r="K1" s="170"/>
+      <c r="L1" s="170"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="166" t="s">
+      <c r="A2" s="167" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="167"/>
-      <c r="C2" s="167"/>
-      <c r="D2" s="167"/>
-      <c r="E2" s="167"/>
-      <c r="F2" s="167"/>
-      <c r="G2" s="167"/>
-      <c r="H2" s="167"/>
-      <c r="I2" s="167"/>
-      <c r="J2" s="167"/>
-      <c r="K2" s="167"/>
-      <c r="L2" s="168"/>
+      <c r="B2" s="168"/>
+      <c r="C2" s="168"/>
+      <c r="D2" s="168"/>
+      <c r="E2" s="168"/>
+      <c r="F2" s="168"/>
+      <c r="G2" s="168"/>
+      <c r="H2" s="168"/>
+      <c r="I2" s="168"/>
+      <c r="J2" s="168"/>
+      <c r="K2" s="168"/>
+      <c r="L2" s="169"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="163" t="s">
+      <c r="A3" s="164" t="s">
         <v>157</v>
       </c>
-      <c r="B3" s="164"/>
-      <c r="C3" s="164"/>
-      <c r="D3" s="164"/>
-      <c r="E3" s="164"/>
-      <c r="F3" s="164"/>
-      <c r="G3" s="164"/>
-      <c r="H3" s="164"/>
-      <c r="I3" s="164"/>
-      <c r="J3" s="164"/>
-      <c r="K3" s="165"/>
+      <c r="B3" s="165"/>
+      <c r="C3" s="165"/>
+      <c r="D3" s="165"/>
+      <c r="E3" s="165"/>
+      <c r="F3" s="165"/>
+      <c r="G3" s="165"/>
+      <c r="H3" s="165"/>
+      <c r="I3" s="165"/>
+      <c r="J3" s="165"/>
+      <c r="K3" s="166"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1">
       <c r="A4" s="28" t="s">
@@ -22767,19 +22789,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A20" s="163" t="s">
+      <c r="A20" s="164" t="s">
         <v>165</v>
       </c>
-      <c r="B20" s="164"/>
-      <c r="C20" s="164"/>
-      <c r="D20" s="164"/>
-      <c r="E20" s="164"/>
-      <c r="F20" s="164"/>
-      <c r="G20" s="164"/>
-      <c r="H20" s="164"/>
-      <c r="I20" s="164"/>
-      <c r="J20" s="164"/>
-      <c r="K20" s="165"/>
+      <c r="B20" s="165"/>
+      <c r="C20" s="165"/>
+      <c r="D20" s="165"/>
+      <c r="E20" s="165"/>
+      <c r="F20" s="165"/>
+      <c r="G20" s="165"/>
+      <c r="H20" s="165"/>
+      <c r="I20" s="165"/>
+      <c r="J20" s="165"/>
+      <c r="K20" s="166"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="28" t="s">
@@ -22996,19 +23018,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A37" s="163" t="s">
+      <c r="A37" s="164" t="s">
         <v>166</v>
       </c>
-      <c r="B37" s="164"/>
-      <c r="C37" s="164"/>
-      <c r="D37" s="164"/>
-      <c r="E37" s="164"/>
-      <c r="F37" s="164"/>
-      <c r="G37" s="164"/>
-      <c r="H37" s="164"/>
-      <c r="I37" s="164"/>
-      <c r="J37" s="164"/>
-      <c r="K37" s="165"/>
+      <c r="B37" s="165"/>
+      <c r="C37" s="165"/>
+      <c r="D37" s="165"/>
+      <c r="E37" s="165"/>
+      <c r="F37" s="165"/>
+      <c r="G37" s="165"/>
+      <c r="H37" s="165"/>
+      <c r="I37" s="165"/>
+      <c r="J37" s="165"/>
+      <c r="K37" s="166"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="28" t="s">
@@ -23232,7 +23254,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -23266,28 +23288,28 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="170"/>
+      <c r="A3" s="171"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="171"/>
+      <c r="A4" s="172"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="171"/>
+      <c r="A5" s="172"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="171"/>
+      <c r="A6" s="172"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="171"/>
+      <c r="A7" s="172"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="171"/>
+      <c r="A8" s="172"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="171"/>
+      <c r="A9" s="172"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1">
-      <c r="A10" s="172"/>
+      <c r="A10" s="173"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1">
       <c r="A11" s="22" t="s">
@@ -23443,7 +23465,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -23470,10 +23492,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="173" t="s">
+      <c r="B1" s="174" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="174"/>
+      <c r="C1" s="175"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -23484,7 +23506,7 @@
       <c r="E2" s="110"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="175" t="s">
+      <c r="A3" s="176" t="s">
         <v>201</v>
       </c>
       <c r="B3" s="118" t="s">
@@ -23498,7 +23520,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="176"/>
+      <c r="A4" s="177"/>
       <c r="B4" s="115" t="s">
         <v>158</v>
       </c>
@@ -23510,7 +23532,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="176"/>
+      <c r="A5" s="177"/>
       <c r="B5" s="115" t="s">
         <v>159</v>
       </c>
@@ -23519,7 +23541,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="176"/>
+      <c r="A6" s="177"/>
       <c r="B6" s="126" t="s">
         <v>203</v>
       </c>
@@ -23531,7 +23553,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="176"/>
+      <c r="A7" s="177"/>
       <c r="B7" s="115" t="s">
         <v>169</v>
       </c>
@@ -23543,7 +23565,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="176"/>
+      <c r="A8" s="177"/>
       <c r="B8" s="115" t="s">
         <v>170</v>
       </c>
@@ -23552,7 +23574,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="177"/>
+      <c r="A9" s="178"/>
       <c r="B9" s="123" t="s">
         <v>160</v>
       </c>
@@ -23567,7 +23589,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="175" t="s">
+      <c r="A11" s="176" t="s">
         <v>202</v>
       </c>
       <c r="B11" s="118" t="s">
@@ -23581,7 +23603,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="176"/>
+      <c r="A12" s="177"/>
       <c r="B12" s="115" t="s">
         <v>158</v>
       </c>
@@ -23593,7 +23615,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="176"/>
+      <c r="A13" s="177"/>
       <c r="B13" s="115" t="s">
         <v>159</v>
       </c>
@@ -23602,7 +23624,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="176"/>
+      <c r="A14" s="177"/>
       <c r="B14" s="126" t="s">
         <v>203</v>
       </c>
@@ -23614,7 +23636,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="176"/>
+      <c r="A15" s="177"/>
       <c r="B15" s="115" t="s">
         <v>169</v>
       </c>
@@ -23626,7 +23648,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="176"/>
+      <c r="A16" s="177"/>
       <c r="B16" s="115" t="s">
         <v>170</v>
       </c>
@@ -23635,7 +23657,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="177"/>
+      <c r="A17" s="178"/>
       <c r="B17" s="123" t="s">
         <v>160</v>
       </c>
@@ -23650,7 +23672,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="175" t="s">
+      <c r="A19" s="176" t="s">
         <v>202</v>
       </c>
       <c r="B19" s="118" t="s">
@@ -23659,7 +23681,7 @@
       <c r="C19" s="117"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="176"/>
+      <c r="A20" s="177"/>
       <c r="B20" s="115" t="s">
         <v>158</v>
       </c>
@@ -23669,14 +23691,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="176"/>
+      <c r="A21" s="177"/>
       <c r="B21" s="115" t="s">
         <v>159</v>
       </c>
       <c r="C21" s="120"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="176"/>
+      <c r="A22" s="177"/>
       <c r="B22" s="126" t="s">
         <v>203</v>
       </c>
@@ -23686,7 +23708,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="176"/>
+      <c r="A23" s="177"/>
       <c r="B23" s="115" t="s">
         <v>169</v>
       </c>
@@ -23696,14 +23718,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="176"/>
+      <c r="A24" s="177"/>
       <c r="B24" s="115" t="s">
         <v>170</v>
       </c>
       <c r="C24" s="119"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="177"/>
+      <c r="A25" s="178"/>
       <c r="B25" s="123" t="s">
         <v>160</v>
       </c>
@@ -23716,7 +23738,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -23747,17 +23769,17 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="194" t="s">
+      <c r="A2" s="185" t="s">
         <v>182</v>
       </c>
-      <c r="B2" s="195"/>
+      <c r="B2" s="186"/>
       <c r="C2" s="111"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="196" t="s">
+      <c r="A3" s="187" t="s">
         <v>184</v>
       </c>
-      <c r="B3" s="195"/>
+      <c r="B3" s="186"/>
       <c r="C3" s="111"/>
     </row>
     <row r="4" spans="1:5">
@@ -23773,115 +23795,128 @@
       <c r="C5" s="111"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="182" t="s">
+      <c r="A7" s="196" t="s">
         <v>185</v>
       </c>
-      <c r="B7" s="183"/>
+      <c r="B7" s="197"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="111"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="184" t="s">
+      <c r="A9" s="194" t="s">
         <v>186</v>
       </c>
-      <c r="B9" s="185"/>
+      <c r="B9" s="195"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="186"/>
-      <c r="B10" s="187"/>
+      <c r="A10" s="181"/>
+      <c r="B10" s="182"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="178" t="s">
+      <c r="A11" s="183" t="s">
         <v>187</v>
       </c>
-      <c r="B11" s="179"/>
+      <c r="B11" s="184"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="178" t="s">
+      <c r="A12" s="183" t="s">
         <v>188</v>
       </c>
-      <c r="B12" s="179"/>
+      <c r="B12" s="184"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="178" t="s">
+      <c r="A13" s="183" t="s">
         <v>189</v>
       </c>
-      <c r="B13" s="179"/>
+      <c r="B13" s="184"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="183" t="s">
         <v>190</v>
       </c>
-      <c r="B14" s="179"/>
+      <c r="B14" s="184"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="178" t="s">
+      <c r="A15" s="183" t="s">
         <v>191</v>
       </c>
-      <c r="B15" s="179"/>
+      <c r="B15" s="184"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="178" t="s">
+      <c r="A16" s="183" t="s">
         <v>192</v>
       </c>
-      <c r="B16" s="179"/>
+      <c r="B16" s="184"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="180" t="s">
+      <c r="A17" s="179" t="s">
         <v>194</v>
       </c>
-      <c r="B17" s="181"/>
+      <c r="B17" s="180"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="182" t="s">
+      <c r="A19" s="196" t="s">
         <v>196</v>
       </c>
-      <c r="B19" s="183"/>
+      <c r="B19" s="197"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="111"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="184" t="s">
+      <c r="A21" s="194" t="s">
         <v>197</v>
       </c>
-      <c r="B21" s="185"/>
+      <c r="B21" s="195"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="186"/>
-      <c r="B22" s="187"/>
+      <c r="A22" s="181"/>
+      <c r="B22" s="182"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="178" t="s">
+      <c r="A23" s="183" t="s">
         <v>198</v>
       </c>
-      <c r="B23" s="179"/>
+      <c r="B23" s="184"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="178"/>
-      <c r="B24" s="179"/>
+      <c r="A24" s="183"/>
+      <c r="B24" s="184"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="178" t="s">
+      <c r="A25" s="183" t="s">
         <v>199</v>
       </c>
-      <c r="B25" s="179"/>
+      <c r="B25" s="184"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="178" t="s">
+      <c r="A26" s="183" t="s">
         <v>200</v>
       </c>
-      <c r="B26" s="179"/>
+      <c r="B26" s="184"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="180"/>
-      <c r="B27" s="181"/>
+      <c r="A27" s="179"/>
+      <c r="B27" s="180"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -23892,19 +23927,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Pit Fighter - big chunk of the game doen 2 fights left, over 5000 frames ahead.
</commit_message>
<xml_diff>
--- a/PitFighter/PitFighter.xlsx
+++ b/PitFighter/PitFighter.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="223">
   <si>
     <t>Notes</t>
   </si>
@@ -699,6 +699,36 @@
   <si>
     <t>Fight 6 begin</t>
   </si>
+  <si>
+    <t>Fight End</t>
+  </si>
+  <si>
+    <t>Fight 7 Begin</t>
+  </si>
+  <si>
+    <t>Fight 7 End</t>
+  </si>
+  <si>
+    <t>Fight 9 Begin</t>
+  </si>
+  <si>
+    <t>Fight 10 Begin</t>
+  </si>
+  <si>
+    <t>Fight 11 Begin</t>
+  </si>
+  <si>
+    <t>Fight 12 begin</t>
+  </si>
+  <si>
+    <t>End Fight</t>
+  </si>
+  <si>
+    <t>Begin Fight 14</t>
+  </si>
+  <si>
+    <t>Begin Fight 13</t>
+  </si>
 </sst>
 </file>
 
@@ -707,10 +737,38 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="46">
+  <fonts count="50">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1596,34 +1654,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1631,185 +1689,182 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="30" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="37" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="28" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="26" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="32" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1819,10 +1874,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1843,95 +1898,108 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="44" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="48" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="48" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="44" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="33" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="33" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="35" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1939,35 +2007,35 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -2278,11 +2346,11 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <pane ySplit="6" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="1"/>
@@ -2298,123 +2366,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="142" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="139" t="s">
+      <c r="B1" s="141"/>
+      <c r="C1" s="143" t="s">
         <v>168</v>
       </c>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="140"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="128">
-        <f>SUM(G1:G65328)</f>
+      <c r="D1" s="143"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="144"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="127">
+        <f>SUM(G1:G65351)</f>
         <v>0</v>
       </c>
-      <c r="I1" s="128" t="s">
+      <c r="I1" s="127" t="s">
         <v>195</v>
       </c>
-      <c r="J1" s="127"/>
-      <c r="K1" s="127"/>
+      <c r="J1" s="126"/>
+      <c r="K1" s="126"/>
     </row>
     <row r="2" spans="1:11" ht="19.5" customHeight="1">
-      <c r="A2" s="129" t="s">
+      <c r="A2" s="128" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="129" t="s">
+      <c r="B2" s="128" t="s">
         <v>179</v>
       </c>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
-      <c r="F2" s="130"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="131">
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="129"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="130">
         <f>IF(H1&lt;3600,H1/60,QUOTIENT(H1, 3600))</f>
         <v>0</v>
       </c>
-      <c r="I2" s="128" t="str">
+      <c r="I2" s="127" t="str">
         <f>IF(H1&lt;3600,"Seconds","Minutes")</f>
         <v>Seconds</v>
       </c>
-      <c r="J2" s="131" t="str">
+      <c r="J2" s="130" t="str">
         <f>IF(H1&lt;3600,"",(MOD(H1,3600)/60))</f>
         <v/>
       </c>
-      <c r="K2" s="128" t="str">
+      <c r="K2" s="127" t="str">
         <f>IF(H1&lt;3600, "", "Seconds")</f>
         <v/>
       </c>
     </row>
     <row r="3" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A3" s="129" t="s">
+      <c r="A3" s="128" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="129" t="s">
+      <c r="B3" s="128" t="s">
         <v>172</v>
       </c>
-      <c r="C3" s="130"/>
-      <c r="D3" s="130"/>
-      <c r="E3" s="130"/>
-      <c r="F3" s="130"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="132"/>
-      <c r="I3" s="127"/>
-      <c r="J3" s="127"/>
-      <c r="K3" s="127"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="126"/>
+      <c r="H3" s="131"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
     </row>
     <row r="4" spans="1:11" ht="8.25" customHeight="1">
-      <c r="A4" s="133"/>
-      <c r="B4" s="133"/>
-      <c r="C4" s="130"/>
-      <c r="D4" s="130"/>
-      <c r="E4" s="130"/>
-      <c r="F4" s="130"/>
-      <c r="G4" s="127"/>
-      <c r="H4" s="127"/>
-      <c r="I4" s="127"/>
-      <c r="J4" s="127"/>
-      <c r="K4" s="127"/>
+      <c r="A4" s="132"/>
+      <c r="B4" s="132"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="126"/>
+      <c r="H4" s="126"/>
+      <c r="I4" s="126"/>
+      <c r="J4" s="126"/>
+      <c r="K4" s="126"/>
     </row>
     <row r="5" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A5" s="134" t="s">
+      <c r="A5" s="133" t="s">
         <v>176</v>
       </c>
-      <c r="B5" s="134" t="s">
+      <c r="B5" s="133" t="s">
         <v>175</v>
       </c>
-      <c r="C5" s="136" t="s">
+      <c r="C5" s="140" t="s">
         <v>177</v>
       </c>
-      <c r="D5" s="136"/>
-      <c r="E5" s="134"/>
-      <c r="F5" s="130"/>
-      <c r="G5" s="127"/>
-      <c r="H5" s="127"/>
-      <c r="I5" s="127"/>
-      <c r="J5" s="127"/>
-      <c r="K5" s="127"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="133"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="126"/>
+      <c r="K5" s="126"/>
     </row>
     <row r="6" spans="1:11" ht="15">
-      <c r="A6" s="134" t="s">
+      <c r="A6" s="133" t="s">
         <v>176</v>
       </c>
-      <c r="B6" s="134" t="s">
+      <c r="B6" s="133" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="136" t="s">
+      <c r="C6" s="140" t="s">
         <v>167</v>
       </c>
-      <c r="D6" s="137"/>
-      <c r="E6" s="134"/>
-      <c r="F6" s="130"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="127"/>
-      <c r="J6" s="127"/>
-      <c r="K6" s="127"/>
+      <c r="D6" s="141"/>
+      <c r="E6" s="133"/>
+      <c r="F6" s="129"/>
+      <c r="G6" s="126"/>
+      <c r="H6" s="126"/>
+      <c r="I6" s="126"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="126"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1">
       <c r="A7" s="93"/>
@@ -2425,7 +2493,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="141" t="s">
+      <c r="A8" s="145" t="s">
         <v>204</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2445,195 +2513,595 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A9" s="142"/>
+      <c r="A9" s="146"/>
       <c r="B9" s="98" t="s">
         <v>175</v>
       </c>
       <c r="C9" s="99"/>
       <c r="D9" s="99"/>
       <c r="E9" s="99"/>
-      <c r="F9" s="104"/>
+      <c r="F9" s="103"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A10" s="142"/>
-      <c r="B10" s="135" t="s">
+      <c r="A10" s="146"/>
+      <c r="B10" s="134" t="s">
         <v>206</v>
       </c>
-      <c r="C10" s="101">
+      <c r="C10" s="100">
         <v>2055</v>
       </c>
-      <c r="D10" s="101">
+      <c r="D10" s="100">
         <v>2991</v>
       </c>
-      <c r="E10" s="101">
-        <f t="shared" ref="E10:E20" si="0">IF(AND(C10&gt;0,D10&gt;0), D10-C10, 0)</f>
+      <c r="E10" s="100">
+        <f t="shared" ref="E10:E43" si="0">IF(AND(C10&gt;0,D10&gt;0), D10-C10, 0)</f>
         <v>936</v>
       </c>
-      <c r="F10" s="105"/>
+      <c r="F10" s="104"/>
     </row>
     <row r="11" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A11" s="142"/>
-      <c r="B11" s="135" t="s">
+      <c r="A11" s="146"/>
+      <c r="B11" s="134" t="s">
         <v>211</v>
       </c>
-      <c r="C11" s="101">
+      <c r="C11" s="100">
         <v>2076</v>
       </c>
-      <c r="D11" s="101">
+      <c r="D11" s="100">
         <v>3023</v>
       </c>
-      <c r="E11" s="101">
+      <c r="E11" s="100">
         <f t="shared" si="0"/>
         <v>947</v>
       </c>
-      <c r="F11" s="105"/>
+      <c r="F11" s="104"/>
     </row>
     <row r="12" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A12" s="142"/>
-      <c r="B12" s="135" t="s">
+      <c r="A12" s="146"/>
+      <c r="B12" s="134" t="s">
         <v>208</v>
       </c>
-      <c r="C12" s="101">
+      <c r="C12" s="100">
         <v>2169</v>
       </c>
-      <c r="D12" s="101">
+      <c r="D12" s="100">
         <v>3096</v>
       </c>
-      <c r="E12" s="101">
+      <c r="E12" s="100">
         <f t="shared" si="0"/>
         <v>927</v>
       </c>
-      <c r="F12" s="105"/>
+      <c r="F12" s="104"/>
     </row>
     <row r="13" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A13" s="142"/>
-      <c r="B13" s="135" t="s">
+      <c r="A13" s="146"/>
+      <c r="B13" s="134" t="s">
         <v>209</v>
       </c>
-      <c r="C13" s="101"/>
-      <c r="D13" s="101">
+      <c r="C13" s="100"/>
+      <c r="D13" s="100">
         <v>3201</v>
       </c>
-      <c r="E13" s="101">
+      <c r="E13" s="100">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F13" s="105"/>
+      <c r="F13" s="104"/>
     </row>
     <row r="14" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A14" s="142"/>
-      <c r="B14" s="135" t="s">
+      <c r="A14" s="146"/>
+      <c r="B14" s="134" t="s">
         <v>210</v>
       </c>
-      <c r="C14" s="101">
+      <c r="C14" s="100">
         <v>2359</v>
       </c>
-      <c r="D14" s="101">
+      <c r="D14" s="100">
         <v>3340</v>
       </c>
-      <c r="E14" s="101">
+      <c r="E14" s="100">
         <f t="shared" si="0"/>
         <v>981</v>
       </c>
-      <c r="F14" s="105"/>
+      <c r="F14" s="104"/>
     </row>
     <row r="15" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A15" s="142"/>
-      <c r="B15" s="198" t="s">
+      <c r="A15" s="146"/>
+      <c r="B15" s="135" t="s">
         <v>212</v>
       </c>
-      <c r="C15" s="101">
+      <c r="C15" s="100">
         <v>5362</v>
       </c>
-      <c r="D15" s="101">
+      <c r="D15" s="100">
         <v>7419</v>
       </c>
-      <c r="E15" s="101">
+      <c r="E15" s="100">
         <f t="shared" si="0"/>
         <v>2057</v>
       </c>
-      <c r="F15" s="105"/>
+      <c r="F15" s="104"/>
     </row>
     <row r="16" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A16" s="142"/>
-      <c r="B16" s="100"/>
-      <c r="C16" s="101"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="105"/>
-    </row>
-    <row r="17" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A17" s="142"/>
-      <c r="B17" s="100"/>
-      <c r="C17" s="101"/>
-      <c r="D17" s="101"/>
-      <c r="E17" s="101">
+      <c r="A16" s="146"/>
+      <c r="B16" s="134" t="s">
+        <v>208</v>
+      </c>
+      <c r="C16" s="100">
+        <v>5462</v>
+      </c>
+      <c r="D16" s="100">
+        <v>7524</v>
+      </c>
+      <c r="E16" s="100">
+        <f t="shared" si="0"/>
+        <v>2062</v>
+      </c>
+      <c r="F16" s="104"/>
+    </row>
+    <row r="17" spans="1:6" ht="15" outlineLevel="1">
+      <c r="A17" s="146"/>
+      <c r="B17" s="134" t="s">
+        <v>209</v>
+      </c>
+      <c r="C17" s="100">
+        <v>5564</v>
+      </c>
+      <c r="D17" s="100">
+        <v>7642</v>
+      </c>
+      <c r="E17" s="100">
+        <f t="shared" si="0"/>
+        <v>2078</v>
+      </c>
+      <c r="F17" s="104"/>
+    </row>
+    <row r="18" spans="1:6" ht="15" outlineLevel="1">
+      <c r="A18" s="146"/>
+      <c r="B18" s="134" t="s">
+        <v>210</v>
+      </c>
+      <c r="C18" s="100">
+        <v>5672</v>
+      </c>
+      <c r="D18" s="100">
+        <v>7774</v>
+      </c>
+      <c r="E18" s="100">
+        <f t="shared" si="0"/>
+        <v>2102</v>
+      </c>
+      <c r="F18" s="104"/>
+    </row>
+    <row r="19" spans="1:6" ht="15" outlineLevel="1">
+      <c r="A19" s="146"/>
+      <c r="B19" s="136" t="s">
+        <v>213</v>
+      </c>
+      <c r="C19" s="137">
+        <v>5907</v>
+      </c>
+      <c r="D19" s="100">
+        <v>8002</v>
+      </c>
+      <c r="E19" s="100">
+        <f t="shared" si="0"/>
+        <v>2095</v>
+      </c>
+      <c r="F19" s="104"/>
+    </row>
+    <row r="20" spans="1:6" ht="15" outlineLevel="1">
+      <c r="A20" s="146"/>
+      <c r="B20" s="136" t="s">
+        <v>214</v>
+      </c>
+      <c r="C20" s="100">
+        <v>6260</v>
+      </c>
+      <c r="D20" s="100">
+        <v>8361</v>
+      </c>
+      <c r="E20" s="100">
+        <f t="shared" si="0"/>
+        <v>2101</v>
+      </c>
+      <c r="F20" s="104"/>
+    </row>
+    <row r="21" spans="1:6" ht="15" outlineLevel="1">
+      <c r="A21" s="146"/>
+      <c r="B21" s="138" t="s">
+        <v>215</v>
+      </c>
+      <c r="C21" s="100">
+        <v>6914</v>
+      </c>
+      <c r="D21" s="100">
+        <v>9370</v>
+      </c>
+      <c r="E21" s="100">
+        <f t="shared" si="0"/>
+        <v>2456</v>
+      </c>
+      <c r="F21" s="104"/>
+    </row>
+    <row r="22" spans="1:6" ht="15" outlineLevel="1">
+      <c r="A22" s="146"/>
+      <c r="B22" s="139" t="s">
+        <v>216</v>
+      </c>
+      <c r="C22" s="100">
+        <v>8370</v>
+      </c>
+      <c r="D22" s="100">
+        <v>11645</v>
+      </c>
+      <c r="E22" s="100">
+        <f t="shared" si="0"/>
+        <v>3275</v>
+      </c>
+      <c r="F22" s="104"/>
+    </row>
+    <row r="23" spans="1:6" ht="15" outlineLevel="1">
+      <c r="A23" s="146"/>
+      <c r="B23" s="139" t="s">
+        <v>208</v>
+      </c>
+      <c r="C23" s="100">
+        <v>8470</v>
+      </c>
+      <c r="D23" s="100">
+        <v>11755</v>
+      </c>
+      <c r="E23" s="100">
+        <f t="shared" si="0"/>
+        <v>3285</v>
+      </c>
+      <c r="F23" s="104"/>
+    </row>
+    <row r="24" spans="1:6" ht="15" outlineLevel="1">
+      <c r="A24" s="146"/>
+      <c r="B24" s="139" t="s">
+        <v>209</v>
+      </c>
+      <c r="C24" s="100">
+        <v>8572</v>
+      </c>
+      <c r="D24" s="100">
+        <v>11839</v>
+      </c>
+      <c r="E24" s="100">
+        <f t="shared" si="0"/>
+        <v>3267</v>
+      </c>
+      <c r="F24" s="104"/>
+    </row>
+    <row r="25" spans="1:6" ht="15" outlineLevel="1">
+      <c r="A25" s="146"/>
+      <c r="B25" s="139" t="s">
+        <v>210</v>
+      </c>
+      <c r="C25" s="100">
+        <v>8680</v>
+      </c>
+      <c r="D25" s="100">
+        <v>11954</v>
+      </c>
+      <c r="E25" s="100">
+        <f t="shared" si="0"/>
+        <v>3274</v>
+      </c>
+      <c r="F25" s="104"/>
+    </row>
+    <row r="26" spans="1:6" ht="15" outlineLevel="1">
+      <c r="A26" s="146"/>
+      <c r="B26" s="139" t="s">
+        <v>213</v>
+      </c>
+      <c r="C26" s="100">
+        <v>9037</v>
+      </c>
+      <c r="D26" s="100">
+        <v>12305</v>
+      </c>
+      <c r="E26" s="100">
+        <f t="shared" si="0"/>
+        <v>3268</v>
+      </c>
+      <c r="F26" s="104"/>
+    </row>
+    <row r="27" spans="1:6" ht="15" outlineLevel="1">
+      <c r="A27" s="146"/>
+      <c r="B27" s="202" t="s">
+        <v>217</v>
+      </c>
+      <c r="C27" s="100">
+        <v>9691</v>
+      </c>
+      <c r="D27" s="100">
+        <v>12967</v>
+      </c>
+      <c r="E27" s="100">
+        <f t="shared" si="0"/>
+        <v>3276</v>
+      </c>
+      <c r="F27" s="104"/>
+    </row>
+    <row r="28" spans="1:6" ht="15" outlineLevel="1">
+      <c r="A28" s="146"/>
+      <c r="B28" s="202" t="s">
+        <v>213</v>
+      </c>
+      <c r="C28" s="100">
+        <v>10352</v>
+      </c>
+      <c r="D28" s="100">
+        <v>14342</v>
+      </c>
+      <c r="E28" s="100">
+        <f t="shared" si="0"/>
+        <v>3990</v>
+      </c>
+      <c r="F28" s="104"/>
+    </row>
+    <row r="29" spans="1:6" ht="15" outlineLevel="1">
+      <c r="A29" s="146"/>
+      <c r="B29" s="202" t="s">
+        <v>218</v>
+      </c>
+      <c r="C29" s="100">
+        <v>10846</v>
+      </c>
+      <c r="D29" s="100">
+        <v>14845</v>
+      </c>
+      <c r="E29" s="100">
+        <f t="shared" si="0"/>
+        <v>3999</v>
+      </c>
+      <c r="F29" s="104"/>
+    </row>
+    <row r="30" spans="1:6" ht="15" outlineLevel="1">
+      <c r="A30" s="146"/>
+      <c r="B30" s="202" t="s">
+        <v>213</v>
+      </c>
+      <c r="C30" s="100">
+        <v>11701</v>
+      </c>
+      <c r="D30" s="100">
+        <v>16106</v>
+      </c>
+      <c r="E30" s="100">
+        <f t="shared" si="0"/>
+        <v>4405</v>
+      </c>
+      <c r="F30" s="104"/>
+    </row>
+    <row r="31" spans="1:6" ht="15" outlineLevel="1">
+      <c r="A31" s="146"/>
+      <c r="B31" s="202" t="s">
+        <v>219</v>
+      </c>
+      <c r="C31" s="100">
+        <v>12189</v>
+      </c>
+      <c r="D31" s="100">
+        <v>16609</v>
+      </c>
+      <c r="E31" s="100">
+        <f t="shared" si="0"/>
+        <v>4420</v>
+      </c>
+      <c r="F31" s="104"/>
+    </row>
+    <row r="32" spans="1:6" ht="15" outlineLevel="1">
+      <c r="A32" s="146"/>
+      <c r="B32" s="134" t="s">
+        <v>208</v>
+      </c>
+      <c r="C32" s="100">
+        <v>12303</v>
+      </c>
+      <c r="D32" s="100">
+        <v>16753</v>
+      </c>
+      <c r="E32" s="100">
+        <f t="shared" si="0"/>
+        <v>4450</v>
+      </c>
+      <c r="F32" s="104"/>
+    </row>
+    <row r="33" spans="1:7" ht="15" outlineLevel="1">
+      <c r="A33" s="146"/>
+      <c r="B33" s="134" t="s">
+        <v>209</v>
+      </c>
+      <c r="C33" s="100">
+        <v>12399</v>
+      </c>
+      <c r="D33" s="100">
+        <v>16849</v>
+      </c>
+      <c r="E33" s="100">
+        <f t="shared" si="0"/>
+        <v>4450</v>
+      </c>
+      <c r="F33" s="104"/>
+    </row>
+    <row r="34" spans="1:7" ht="15" outlineLevel="1">
+      <c r="A34" s="146"/>
+      <c r="B34" s="134" t="s">
+        <v>210</v>
+      </c>
+      <c r="C34" s="100">
+        <v>12516</v>
+      </c>
+      <c r="D34" s="100">
+        <v>16999</v>
+      </c>
+      <c r="E34" s="100">
+        <f t="shared" si="0"/>
+        <v>4483</v>
+      </c>
+      <c r="F34" s="104"/>
+    </row>
+    <row r="35" spans="1:7" ht="15" outlineLevel="1">
+      <c r="A35" s="146"/>
+      <c r="B35" s="202" t="s">
+        <v>220</v>
+      </c>
+      <c r="C35" s="100">
+        <v>12754</v>
+      </c>
+      <c r="D35" s="100">
+        <v>17231</v>
+      </c>
+      <c r="E35" s="100">
+        <f t="shared" si="0"/>
+        <v>4477</v>
+      </c>
+      <c r="F35" s="104"/>
+    </row>
+    <row r="36" spans="1:7" ht="15" outlineLevel="1">
+      <c r="A36" s="146"/>
+      <c r="B36" s="202" t="s">
+        <v>222</v>
+      </c>
+      <c r="C36" s="100">
+        <v>13492</v>
+      </c>
+      <c r="D36" s="100">
+        <v>17975</v>
+      </c>
+      <c r="E36" s="100">
+        <f t="shared" si="0"/>
+        <v>4483</v>
+      </c>
+      <c r="F36" s="104"/>
+    </row>
+    <row r="37" spans="1:7" ht="15" outlineLevel="1">
+      <c r="A37" s="146"/>
+      <c r="B37" s="202" t="s">
+        <v>220</v>
+      </c>
+      <c r="C37" s="100">
+        <v>14186</v>
+      </c>
+      <c r="D37" s="100">
+        <v>19008</v>
+      </c>
+      <c r="E37" s="100">
+        <f t="shared" si="0"/>
+        <v>4822</v>
+      </c>
+      <c r="F37" s="104"/>
+    </row>
+    <row r="38" spans="1:7" ht="15" outlineLevel="1">
+      <c r="A38" s="146"/>
+      <c r="B38" s="202" t="s">
+        <v>221</v>
+      </c>
+      <c r="C38" s="100">
+        <v>14807</v>
+      </c>
+      <c r="D38" s="100">
+        <v>19633</v>
+      </c>
+      <c r="E38" s="100">
+        <f t="shared" si="0"/>
+        <v>4826</v>
+      </c>
+      <c r="F38" s="104"/>
+    </row>
+    <row r="39" spans="1:7" ht="15" outlineLevel="1">
+      <c r="A39" s="146"/>
+      <c r="B39" s="202" t="s">
+        <v>220</v>
+      </c>
+      <c r="C39" s="100">
+        <v>16658</v>
+      </c>
+      <c r="D39" s="100">
+        <v>21722</v>
+      </c>
+      <c r="E39" s="100">
+        <f t="shared" si="0"/>
+        <v>5064</v>
+      </c>
+      <c r="F39" s="104"/>
+    </row>
+    <row r="40" spans="1:7" ht="15" outlineLevel="1">
+      <c r="A40" s="146"/>
+      <c r="B40" s="202"/>
+      <c r="C40" s="100"/>
+      <c r="D40" s="100"/>
+      <c r="E40" s="100">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F17" s="105"/>
-    </row>
-    <row r="18" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A18" s="142"/>
-      <c r="B18" s="100"/>
-      <c r="C18" s="101"/>
-      <c r="D18" s="101"/>
-      <c r="E18" s="101">
+      <c r="F40" s="104"/>
+    </row>
+    <row r="41" spans="1:7" ht="15" outlineLevel="1">
+      <c r="A41" s="146"/>
+      <c r="B41" s="134"/>
+      <c r="C41" s="100"/>
+      <c r="D41" s="100"/>
+      <c r="E41" s="100">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F18" s="105"/>
-    </row>
-    <row r="19" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A19" s="142"/>
-      <c r="B19" s="100"/>
-      <c r="C19" s="101"/>
-      <c r="D19" s="101"/>
-      <c r="E19" s="112">
+      <c r="F41" s="104"/>
+    </row>
+    <row r="42" spans="1:7" ht="15" outlineLevel="1">
+      <c r="A42" s="146"/>
+      <c r="B42" s="134"/>
+      <c r="C42" s="100"/>
+      <c r="D42" s="100"/>
+      <c r="E42" s="111">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F19" s="105"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A20" s="142"/>
-      <c r="B20" s="98" t="s">
+      <c r="F42" s="104"/>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A43" s="146"/>
+      <c r="B43" s="98" t="s">
         <v>178</v>
       </c>
-      <c r="C20" s="99">
+      <c r="C43" s="99">
         <v>0</v>
       </c>
-      <c r="D20" s="99">
+      <c r="D43" s="99">
         <v>0</v>
       </c>
-      <c r="E20" s="101">
+      <c r="E43" s="100">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F20" s="104"/>
-    </row>
-    <row r="21" spans="1:7" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A21" s="108" t="s">
+      <c r="F43" s="103"/>
+    </row>
+    <row r="44" spans="1:7" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A44" s="107" t="s">
         <v>205</v>
       </c>
-      <c r="B21" s="102" t="s">
+      <c r="B44" s="101" t="s">
         <v>180</v>
       </c>
-      <c r="C21" s="103">
-        <f>C20-C9</f>
+      <c r="C44" s="102">
+        <f>C43-C9</f>
         <v>0</v>
       </c>
-      <c r="D21" s="103">
-        <f>D20-D9</f>
+      <c r="D44" s="102">
+        <f>D43-D9</f>
         <v>0</v>
       </c>
-      <c r="E21" s="113">
-        <f>E20-E9</f>
+      <c r="E44" s="112">
+        <f>E43-E9</f>
         <v>0</v>
       </c>
-      <c r="F21" s="106"/>
-      <c r="G21" s="107">
-        <f>E21</f>
+      <c r="F44" s="105"/>
+      <c r="G44" s="106">
+        <f>E44</f>
         <v>0</v>
       </c>
     </row>
@@ -2643,7 +3111,7 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A8:A20"/>
+    <mergeCell ref="A8:A43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2675,13 +3143,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="165" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
+      <c r="B1" s="165"/>
+      <c r="C1" s="165"/>
+      <c r="D1" s="165"/>
+      <c r="E1" s="165"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -2711,18 +3179,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="162"/>
-      <c r="D3" s="163"/>
-      <c r="E3" s="163"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="167"/>
+      <c r="E3" s="167"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="143"/>
-      <c r="D4" s="144"/>
-      <c r="E4" s="144"/>
+      <c r="C4" s="147"/>
+      <c r="D4" s="148"/>
+      <c r="E4" s="148"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -2874,9 +3342,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="145"/>
-      <c r="D21" s="146"/>
-      <c r="E21" s="146"/>
+      <c r="C21" s="149"/>
+      <c r="D21" s="150"/>
+      <c r="E21" s="150"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -3027,9 +3495,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="143"/>
-      <c r="D38" s="144"/>
-      <c r="E38" s="144"/>
+      <c r="C38" s="147"/>
+      <c r="D38" s="148"/>
+      <c r="E38" s="148"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -3180,9 +3648,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="143"/>
-      <c r="D55" s="144"/>
-      <c r="E55" s="144"/>
+      <c r="C55" s="147"/>
+      <c r="D55" s="148"/>
+      <c r="E55" s="148"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -3333,9 +3801,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="143"/>
-      <c r="D72" s="144"/>
-      <c r="E72" s="144"/>
+      <c r="C72" s="147"/>
+      <c r="D72" s="148"/>
+      <c r="E72" s="148"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -3486,9 +3954,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="143"/>
-      <c r="D89" s="144"/>
-      <c r="E89" s="144"/>
+      <c r="C89" s="147"/>
+      <c r="D89" s="148"/>
+      <c r="E89" s="148"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -3639,9 +4107,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="143"/>
-      <c r="D106" s="144"/>
-      <c r="E106" s="144"/>
+      <c r="C106" s="147"/>
+      <c r="D106" s="148"/>
+      <c r="E106" s="148"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -3792,9 +4260,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="143"/>
-      <c r="D123" s="144"/>
-      <c r="E123" s="144"/>
+      <c r="C123" s="147"/>
+      <c r="D123" s="148"/>
+      <c r="E123" s="148"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -3945,9 +4413,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="143"/>
-      <c r="D140" s="144"/>
-      <c r="E140" s="144"/>
+      <c r="C140" s="147"/>
+      <c r="D140" s="148"/>
+      <c r="E140" s="148"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -4098,9 +4566,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="143"/>
-      <c r="D157" s="144"/>
-      <c r="E157" s="144"/>
+      <c r="C157" s="147"/>
+      <c r="D157" s="148"/>
+      <c r="E157" s="148"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -4251,9 +4719,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="143"/>
-      <c r="D174" s="144"/>
-      <c r="E174" s="144"/>
+      <c r="C174" s="147"/>
+      <c r="D174" s="148"/>
+      <c r="E174" s="148"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -4404,9 +4872,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="143"/>
-      <c r="D191" s="144"/>
-      <c r="E191" s="144"/>
+      <c r="C191" s="147"/>
+      <c r="D191" s="148"/>
+      <c r="E191" s="148"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -4557,9 +5025,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="143"/>
-      <c r="D208" s="144"/>
-      <c r="E208" s="144"/>
+      <c r="C208" s="147"/>
+      <c r="D208" s="148"/>
+      <c r="E208" s="148"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -4710,9 +5178,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="143"/>
-      <c r="D225" s="144"/>
-      <c r="E225" s="144"/>
+      <c r="C225" s="147"/>
+      <c r="D225" s="148"/>
+      <c r="E225" s="148"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -4863,9 +5331,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="143"/>
-      <c r="D242" s="144"/>
-      <c r="E242" s="144"/>
+      <c r="C242" s="147"/>
+      <c r="D242" s="148"/>
+      <c r="E242" s="148"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -5016,9 +5484,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="143"/>
-      <c r="D259" s="144"/>
-      <c r="E259" s="144"/>
+      <c r="C259" s="147"/>
+      <c r="D259" s="148"/>
+      <c r="E259" s="148"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -5169,18 +5637,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="159"/>
-      <c r="D276" s="160"/>
-      <c r="E276" s="160"/>
+      <c r="C276" s="163"/>
+      <c r="D276" s="164"/>
+      <c r="E276" s="164"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="143"/>
-      <c r="D277" s="144"/>
-      <c r="E277" s="144"/>
+      <c r="C277" s="147"/>
+      <c r="D277" s="148"/>
+      <c r="E277" s="148"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -5331,9 +5799,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="145"/>
-      <c r="D294" s="146"/>
-      <c r="E294" s="146"/>
+      <c r="C294" s="149"/>
+      <c r="D294" s="150"/>
+      <c r="E294" s="150"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -5484,9 +5952,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="143"/>
-      <c r="D311" s="144"/>
-      <c r="E311" s="144"/>
+      <c r="C311" s="147"/>
+      <c r="D311" s="148"/>
+      <c r="E311" s="148"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -5637,9 +6105,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="143"/>
-      <c r="D328" s="144"/>
-      <c r="E328" s="144"/>
+      <c r="C328" s="147"/>
+      <c r="D328" s="148"/>
+      <c r="E328" s="148"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -5790,9 +6258,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="143"/>
-      <c r="D345" s="144"/>
-      <c r="E345" s="144"/>
+      <c r="C345" s="147"/>
+      <c r="D345" s="148"/>
+      <c r="E345" s="148"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -5943,9 +6411,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="143"/>
-      <c r="D362" s="144"/>
-      <c r="E362" s="144"/>
+      <c r="C362" s="147"/>
+      <c r="D362" s="148"/>
+      <c r="E362" s="148"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -6096,9 +6564,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="143"/>
-      <c r="D379" s="144"/>
-      <c r="E379" s="144"/>
+      <c r="C379" s="147"/>
+      <c r="D379" s="148"/>
+      <c r="E379" s="148"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -6249,9 +6717,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="143"/>
-      <c r="D396" s="144"/>
-      <c r="E396" s="144"/>
+      <c r="C396" s="147"/>
+      <c r="D396" s="148"/>
+      <c r="E396" s="148"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -6402,9 +6870,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="143"/>
-      <c r="D413" s="144"/>
-      <c r="E413" s="144"/>
+      <c r="C413" s="147"/>
+      <c r="D413" s="148"/>
+      <c r="E413" s="148"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -6555,9 +7023,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="143"/>
-      <c r="D430" s="144"/>
-      <c r="E430" s="144"/>
+      <c r="C430" s="147"/>
+      <c r="D430" s="148"/>
+      <c r="E430" s="148"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -6708,9 +7176,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="143"/>
-      <c r="D447" s="144"/>
-      <c r="E447" s="144"/>
+      <c r="C447" s="147"/>
+      <c r="D447" s="148"/>
+      <c r="E447" s="148"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -6861,9 +7329,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="143"/>
-      <c r="D464" s="144"/>
-      <c r="E464" s="144"/>
+      <c r="C464" s="147"/>
+      <c r="D464" s="148"/>
+      <c r="E464" s="148"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -7014,9 +7482,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="143"/>
-      <c r="D481" s="144"/>
-      <c r="E481" s="144"/>
+      <c r="C481" s="147"/>
+      <c r="D481" s="148"/>
+      <c r="E481" s="148"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -7167,9 +7635,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="143"/>
-      <c r="D498" s="144"/>
-      <c r="E498" s="144"/>
+      <c r="C498" s="147"/>
+      <c r="D498" s="148"/>
+      <c r="E498" s="148"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -7320,9 +7788,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="143"/>
-      <c r="D515" s="144"/>
-      <c r="E515" s="144"/>
+      <c r="C515" s="147"/>
+      <c r="D515" s="148"/>
+      <c r="E515" s="148"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -7473,9 +7941,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="143"/>
-      <c r="D532" s="144"/>
-      <c r="E532" s="144"/>
+      <c r="C532" s="147"/>
+      <c r="D532" s="148"/>
+      <c r="E532" s="148"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -7626,18 +8094,18 @@
         <v>49</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="157"/>
-      <c r="D549" s="158"/>
-      <c r="E549" s="158"/>
+      <c r="C549" s="161"/>
+      <c r="D549" s="162"/>
+      <c r="E549" s="162"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>50</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="143"/>
-      <c r="D550" s="144"/>
-      <c r="E550" s="144"/>
+      <c r="C550" s="147"/>
+      <c r="D550" s="148"/>
+      <c r="E550" s="148"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -7788,9 +8256,9 @@
         <v>51</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="145"/>
-      <c r="D567" s="146"/>
-      <c r="E567" s="146"/>
+      <c r="C567" s="149"/>
+      <c r="D567" s="150"/>
+      <c r="E567" s="150"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -7941,9 +8409,9 @@
         <v>52</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="143"/>
-      <c r="D584" s="144"/>
-      <c r="E584" s="144"/>
+      <c r="C584" s="147"/>
+      <c r="D584" s="148"/>
+      <c r="E584" s="148"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -8094,9 +8562,9 @@
         <v>53</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="143"/>
-      <c r="D601" s="144"/>
-      <c r="E601" s="144"/>
+      <c r="C601" s="147"/>
+      <c r="D601" s="148"/>
+      <c r="E601" s="148"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -8247,9 +8715,9 @@
         <v>54</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="143"/>
-      <c r="D618" s="144"/>
-      <c r="E618" s="144"/>
+      <c r="C618" s="147"/>
+      <c r="D618" s="148"/>
+      <c r="E618" s="148"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -8400,9 +8868,9 @@
         <v>55</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="143"/>
-      <c r="D635" s="144"/>
-      <c r="E635" s="144"/>
+      <c r="C635" s="147"/>
+      <c r="D635" s="148"/>
+      <c r="E635" s="148"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -8553,9 +9021,9 @@
         <v>56</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="143"/>
-      <c r="D652" s="144"/>
-      <c r="E652" s="144"/>
+      <c r="C652" s="147"/>
+      <c r="D652" s="148"/>
+      <c r="E652" s="148"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -8706,9 +9174,9 @@
         <v>57</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="143"/>
-      <c r="D669" s="144"/>
-      <c r="E669" s="144"/>
+      <c r="C669" s="147"/>
+      <c r="D669" s="148"/>
+      <c r="E669" s="148"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -8859,9 +9327,9 @@
         <v>58</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="143"/>
-      <c r="D686" s="144"/>
-      <c r="E686" s="144"/>
+      <c r="C686" s="147"/>
+      <c r="D686" s="148"/>
+      <c r="E686" s="148"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -9012,9 +9480,9 @@
         <v>59</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="143"/>
-      <c r="D703" s="144"/>
-      <c r="E703" s="144"/>
+      <c r="C703" s="147"/>
+      <c r="D703" s="148"/>
+      <c r="E703" s="148"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -9165,9 +9633,9 @@
         <v>60</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="143"/>
-      <c r="D720" s="144"/>
-      <c r="E720" s="144"/>
+      <c r="C720" s="147"/>
+      <c r="D720" s="148"/>
+      <c r="E720" s="148"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -9318,9 +9786,9 @@
         <v>61</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="143"/>
-      <c r="D737" s="144"/>
-      <c r="E737" s="144"/>
+      <c r="C737" s="147"/>
+      <c r="D737" s="148"/>
+      <c r="E737" s="148"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -9471,9 +9939,9 @@
         <v>62</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="143"/>
-      <c r="D754" s="144"/>
-      <c r="E754" s="144"/>
+      <c r="C754" s="147"/>
+      <c r="D754" s="148"/>
+      <c r="E754" s="148"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -9624,9 +10092,9 @@
         <v>63</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="143"/>
-      <c r="D771" s="144"/>
-      <c r="E771" s="144"/>
+      <c r="C771" s="147"/>
+      <c r="D771" s="148"/>
+      <c r="E771" s="148"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -9777,9 +10245,9 @@
         <v>64</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="143"/>
-      <c r="D788" s="144"/>
-      <c r="E788" s="144"/>
+      <c r="C788" s="147"/>
+      <c r="D788" s="148"/>
+      <c r="E788" s="148"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -9930,9 +10398,9 @@
         <v>65</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="143"/>
-      <c r="D805" s="144"/>
-      <c r="E805" s="144"/>
+      <c r="C805" s="147"/>
+      <c r="D805" s="148"/>
+      <c r="E805" s="148"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -10083,18 +10551,18 @@
         <v>66</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="155"/>
-      <c r="D822" s="156"/>
-      <c r="E822" s="156"/>
+      <c r="C822" s="159"/>
+      <c r="D822" s="160"/>
+      <c r="E822" s="160"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>67</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="143"/>
-      <c r="D823" s="144"/>
-      <c r="E823" s="144"/>
+      <c r="C823" s="147"/>
+      <c r="D823" s="148"/>
+      <c r="E823" s="148"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -10245,9 +10713,9 @@
         <v>68</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="145"/>
-      <c r="D840" s="146"/>
-      <c r="E840" s="146"/>
+      <c r="C840" s="149"/>
+      <c r="D840" s="150"/>
+      <c r="E840" s="150"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -10398,9 +10866,9 @@
         <v>69</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="143"/>
-      <c r="D857" s="144"/>
-      <c r="E857" s="144"/>
+      <c r="C857" s="147"/>
+      <c r="D857" s="148"/>
+      <c r="E857" s="148"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -10551,9 +11019,9 @@
         <v>70</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="143"/>
-      <c r="D874" s="144"/>
-      <c r="E874" s="144"/>
+      <c r="C874" s="147"/>
+      <c r="D874" s="148"/>
+      <c r="E874" s="148"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -10704,9 +11172,9 @@
         <v>71</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="143"/>
-      <c r="D891" s="144"/>
-      <c r="E891" s="144"/>
+      <c r="C891" s="147"/>
+      <c r="D891" s="148"/>
+      <c r="E891" s="148"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -10857,9 +11325,9 @@
         <v>72</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="143"/>
-      <c r="D908" s="144"/>
-      <c r="E908" s="144"/>
+      <c r="C908" s="147"/>
+      <c r="D908" s="148"/>
+      <c r="E908" s="148"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -11010,9 +11478,9 @@
         <v>73</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="143"/>
-      <c r="D925" s="144"/>
-      <c r="E925" s="144"/>
+      <c r="C925" s="147"/>
+      <c r="D925" s="148"/>
+      <c r="E925" s="148"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -11163,9 +11631,9 @@
         <v>74</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="143"/>
-      <c r="D942" s="144"/>
-      <c r="E942" s="144"/>
+      <c r="C942" s="147"/>
+      <c r="D942" s="148"/>
+      <c r="E942" s="148"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -11316,9 +11784,9 @@
         <v>75</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="143"/>
-      <c r="D959" s="144"/>
-      <c r="E959" s="144"/>
+      <c r="C959" s="147"/>
+      <c r="D959" s="148"/>
+      <c r="E959" s="148"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -11469,9 +11937,9 @@
         <v>76</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="143"/>
-      <c r="D976" s="144"/>
-      <c r="E976" s="144"/>
+      <c r="C976" s="147"/>
+      <c r="D976" s="148"/>
+      <c r="E976" s="148"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -11622,9 +12090,9 @@
         <v>77</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="143"/>
-      <c r="D993" s="144"/>
-      <c r="E993" s="144"/>
+      <c r="C993" s="147"/>
+      <c r="D993" s="148"/>
+      <c r="E993" s="148"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -11775,9 +12243,9 @@
         <v>78</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="143"/>
-      <c r="D1010" s="144"/>
-      <c r="E1010" s="144"/>
+      <c r="C1010" s="147"/>
+      <c r="D1010" s="148"/>
+      <c r="E1010" s="148"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -11928,9 +12396,9 @@
         <v>79</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="143"/>
-      <c r="D1027" s="144"/>
-      <c r="E1027" s="144"/>
+      <c r="C1027" s="147"/>
+      <c r="D1027" s="148"/>
+      <c r="E1027" s="148"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -12081,9 +12549,9 @@
         <v>82</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="143"/>
-      <c r="D1044" s="144"/>
-      <c r="E1044" s="144"/>
+      <c r="C1044" s="147"/>
+      <c r="D1044" s="148"/>
+      <c r="E1044" s="148"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -12234,9 +12702,9 @@
         <v>81</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="143"/>
-      <c r="D1061" s="144"/>
-      <c r="E1061" s="144"/>
+      <c r="C1061" s="147"/>
+      <c r="D1061" s="148"/>
+      <c r="E1061" s="148"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -12387,9 +12855,9 @@
         <v>83</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="143"/>
-      <c r="D1078" s="144"/>
-      <c r="E1078" s="144"/>
+      <c r="C1078" s="147"/>
+      <c r="D1078" s="148"/>
+      <c r="E1078" s="148"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -12540,18 +13008,18 @@
         <v>103</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="153"/>
-      <c r="D1095" s="154"/>
-      <c r="E1095" s="154"/>
+      <c r="C1095" s="157"/>
+      <c r="D1095" s="158"/>
+      <c r="E1095" s="158"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>84</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="143"/>
-      <c r="D1096" s="144"/>
-      <c r="E1096" s="144"/>
+      <c r="C1096" s="147"/>
+      <c r="D1096" s="148"/>
+      <c r="E1096" s="148"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -12702,9 +13170,9 @@
         <v>85</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="145"/>
-      <c r="D1113" s="146"/>
-      <c r="E1113" s="146"/>
+      <c r="C1113" s="149"/>
+      <c r="D1113" s="150"/>
+      <c r="E1113" s="150"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -12855,9 +13323,9 @@
         <v>86</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="143"/>
-      <c r="D1130" s="144"/>
-      <c r="E1130" s="144"/>
+      <c r="C1130" s="147"/>
+      <c r="D1130" s="148"/>
+      <c r="E1130" s="148"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -13008,9 +13476,9 @@
         <v>87</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="143"/>
-      <c r="D1147" s="144"/>
-      <c r="E1147" s="144"/>
+      <c r="C1147" s="147"/>
+      <c r="D1147" s="148"/>
+      <c r="E1147" s="148"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -13161,9 +13629,9 @@
         <v>88</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="143"/>
-      <c r="D1164" s="144"/>
-      <c r="E1164" s="144"/>
+      <c r="C1164" s="147"/>
+      <c r="D1164" s="148"/>
+      <c r="E1164" s="148"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -13314,9 +13782,9 @@
         <v>89</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="143"/>
-      <c r="D1181" s="144"/>
-      <c r="E1181" s="144"/>
+      <c r="C1181" s="147"/>
+      <c r="D1181" s="148"/>
+      <c r="E1181" s="148"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -13467,9 +13935,9 @@
         <v>90</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="143"/>
-      <c r="D1198" s="144"/>
-      <c r="E1198" s="144"/>
+      <c r="C1198" s="147"/>
+      <c r="D1198" s="148"/>
+      <c r="E1198" s="148"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -13620,9 +14088,9 @@
         <v>91</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="143"/>
-      <c r="D1215" s="144"/>
-      <c r="E1215" s="144"/>
+      <c r="C1215" s="147"/>
+      <c r="D1215" s="148"/>
+      <c r="E1215" s="148"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -13773,9 +14241,9 @@
         <v>92</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="143"/>
-      <c r="D1232" s="144"/>
-      <c r="E1232" s="144"/>
+      <c r="C1232" s="147"/>
+      <c r="D1232" s="148"/>
+      <c r="E1232" s="148"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -13926,9 +14394,9 @@
         <v>93</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="143"/>
-      <c r="D1249" s="144"/>
-      <c r="E1249" s="144"/>
+      <c r="C1249" s="147"/>
+      <c r="D1249" s="148"/>
+      <c r="E1249" s="148"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -14079,9 +14547,9 @@
         <v>98</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="143"/>
-      <c r="D1266" s="144"/>
-      <c r="E1266" s="144"/>
+      <c r="C1266" s="147"/>
+      <c r="D1266" s="148"/>
+      <c r="E1266" s="148"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -14232,9 +14700,9 @@
         <v>99</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="143"/>
-      <c r="D1283" s="144"/>
-      <c r="E1283" s="144"/>
+      <c r="C1283" s="147"/>
+      <c r="D1283" s="148"/>
+      <c r="E1283" s="148"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -14385,9 +14853,9 @@
         <v>100</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="143"/>
-      <c r="D1300" s="144"/>
-      <c r="E1300" s="144"/>
+      <c r="C1300" s="147"/>
+      <c r="D1300" s="148"/>
+      <c r="E1300" s="148"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -14538,9 +15006,9 @@
         <v>80</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="143"/>
-      <c r="D1317" s="144"/>
-      <c r="E1317" s="144"/>
+      <c r="C1317" s="147"/>
+      <c r="D1317" s="148"/>
+      <c r="E1317" s="148"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -14691,9 +15159,9 @@
         <v>101</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="143"/>
-      <c r="D1334" s="144"/>
-      <c r="E1334" s="144"/>
+      <c r="C1334" s="147"/>
+      <c r="D1334" s="148"/>
+      <c r="E1334" s="148"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -14844,9 +15312,9 @@
         <v>97</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="143"/>
-      <c r="D1351" s="144"/>
-      <c r="E1351" s="144"/>
+      <c r="C1351" s="147"/>
+      <c r="D1351" s="148"/>
+      <c r="E1351" s="148"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -14997,18 +15465,18 @@
         <v>102</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="151"/>
-      <c r="D1368" s="152"/>
-      <c r="E1368" s="152"/>
+      <c r="C1368" s="155"/>
+      <c r="D1368" s="156"/>
+      <c r="E1368" s="156"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>104</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="143"/>
-      <c r="D1369" s="144"/>
-      <c r="E1369" s="144"/>
+      <c r="C1369" s="147"/>
+      <c r="D1369" s="148"/>
+      <c r="E1369" s="148"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -15159,9 +15627,9 @@
         <v>105</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="145"/>
-      <c r="D1386" s="146"/>
-      <c r="E1386" s="146"/>
+      <c r="C1386" s="149"/>
+      <c r="D1386" s="150"/>
+      <c r="E1386" s="150"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -15312,9 +15780,9 @@
         <v>106</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="143"/>
-      <c r="D1403" s="144"/>
-      <c r="E1403" s="144"/>
+      <c r="C1403" s="147"/>
+      <c r="D1403" s="148"/>
+      <c r="E1403" s="148"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -15465,9 +15933,9 @@
         <v>107</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="143"/>
-      <c r="D1420" s="144"/>
-      <c r="E1420" s="144"/>
+      <c r="C1420" s="147"/>
+      <c r="D1420" s="148"/>
+      <c r="E1420" s="148"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -15618,9 +16086,9 @@
         <v>108</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="143"/>
-      <c r="D1437" s="144"/>
-      <c r="E1437" s="144"/>
+      <c r="C1437" s="147"/>
+      <c r="D1437" s="148"/>
+      <c r="E1437" s="148"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -15771,9 +16239,9 @@
         <v>109</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="143"/>
-      <c r="D1454" s="144"/>
-      <c r="E1454" s="144"/>
+      <c r="C1454" s="147"/>
+      <c r="D1454" s="148"/>
+      <c r="E1454" s="148"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -15924,9 +16392,9 @@
         <v>110</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="143"/>
-      <c r="D1471" s="144"/>
-      <c r="E1471" s="144"/>
+      <c r="C1471" s="147"/>
+      <c r="D1471" s="148"/>
+      <c r="E1471" s="148"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -16077,9 +16545,9 @@
         <v>111</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="143"/>
-      <c r="D1488" s="144"/>
-      <c r="E1488" s="144"/>
+      <c r="C1488" s="147"/>
+      <c r="D1488" s="148"/>
+      <c r="E1488" s="148"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -16230,9 +16698,9 @@
         <v>112</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="143"/>
-      <c r="D1505" s="144"/>
-      <c r="E1505" s="144"/>
+      <c r="C1505" s="147"/>
+      <c r="D1505" s="148"/>
+      <c r="E1505" s="148"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -16383,9 +16851,9 @@
         <v>113</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="143"/>
-      <c r="D1522" s="144"/>
-      <c r="E1522" s="144"/>
+      <c r="C1522" s="147"/>
+      <c r="D1522" s="148"/>
+      <c r="E1522" s="148"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -16536,9 +17004,9 @@
         <v>94</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="143"/>
-      <c r="D1539" s="144"/>
-      <c r="E1539" s="144"/>
+      <c r="C1539" s="147"/>
+      <c r="D1539" s="148"/>
+      <c r="E1539" s="148"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -16689,9 +17157,9 @@
         <v>114</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="143"/>
-      <c r="D1556" s="144"/>
-      <c r="E1556" s="144"/>
+      <c r="C1556" s="147"/>
+      <c r="D1556" s="148"/>
+      <c r="E1556" s="148"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -16842,9 +17310,9 @@
         <v>115</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="143"/>
-      <c r="D1573" s="144"/>
-      <c r="E1573" s="144"/>
+      <c r="C1573" s="147"/>
+      <c r="D1573" s="148"/>
+      <c r="E1573" s="148"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -16995,9 +17463,9 @@
         <v>116</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="143"/>
-      <c r="D1590" s="144"/>
-      <c r="E1590" s="144"/>
+      <c r="C1590" s="147"/>
+      <c r="D1590" s="148"/>
+      <c r="E1590" s="148"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -17148,9 +17616,9 @@
         <v>117</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="143"/>
-      <c r="D1607" s="144"/>
-      <c r="E1607" s="144"/>
+      <c r="C1607" s="147"/>
+      <c r="D1607" s="148"/>
+      <c r="E1607" s="148"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -17301,9 +17769,9 @@
         <v>118</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="143"/>
-      <c r="D1624" s="144"/>
-      <c r="E1624" s="144"/>
+      <c r="C1624" s="147"/>
+      <c r="D1624" s="148"/>
+      <c r="E1624" s="148"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -17454,18 +17922,18 @@
         <v>119</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="149"/>
-      <c r="D1641" s="150"/>
-      <c r="E1641" s="150"/>
+      <c r="C1641" s="153"/>
+      <c r="D1641" s="154"/>
+      <c r="E1641" s="154"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>120</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="143"/>
-      <c r="D1642" s="144"/>
-      <c r="E1642" s="144"/>
+      <c r="C1642" s="147"/>
+      <c r="D1642" s="148"/>
+      <c r="E1642" s="148"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -17616,9 +18084,9 @@
         <v>121</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="145"/>
-      <c r="D1659" s="146"/>
-      <c r="E1659" s="146"/>
+      <c r="C1659" s="149"/>
+      <c r="D1659" s="150"/>
+      <c r="E1659" s="150"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -17769,9 +18237,9 @@
         <v>122</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="143"/>
-      <c r="D1676" s="144"/>
-      <c r="E1676" s="144"/>
+      <c r="C1676" s="147"/>
+      <c r="D1676" s="148"/>
+      <c r="E1676" s="148"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -17922,9 +18390,9 @@
         <v>123</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="143"/>
-      <c r="D1693" s="144"/>
-      <c r="E1693" s="144"/>
+      <c r="C1693" s="147"/>
+      <c r="D1693" s="148"/>
+      <c r="E1693" s="148"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -18075,9 +18543,9 @@
         <v>124</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="143"/>
-      <c r="D1710" s="144"/>
-      <c r="E1710" s="144"/>
+      <c r="C1710" s="147"/>
+      <c r="D1710" s="148"/>
+      <c r="E1710" s="148"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -18228,9 +18696,9 @@
         <v>125</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="143"/>
-      <c r="D1727" s="144"/>
-      <c r="E1727" s="144"/>
+      <c r="C1727" s="147"/>
+      <c r="D1727" s="148"/>
+      <c r="E1727" s="148"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -18381,9 +18849,9 @@
         <v>126</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="143"/>
-      <c r="D1744" s="144"/>
-      <c r="E1744" s="144"/>
+      <c r="C1744" s="147"/>
+      <c r="D1744" s="148"/>
+      <c r="E1744" s="148"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -18534,9 +19002,9 @@
         <v>127</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="143"/>
-      <c r="D1761" s="144"/>
-      <c r="E1761" s="144"/>
+      <c r="C1761" s="147"/>
+      <c r="D1761" s="148"/>
+      <c r="E1761" s="148"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -18687,9 +19155,9 @@
         <v>128</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="143"/>
-      <c r="D1778" s="144"/>
-      <c r="E1778" s="144"/>
+      <c r="C1778" s="147"/>
+      <c r="D1778" s="148"/>
+      <c r="E1778" s="148"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -18840,9 +19308,9 @@
         <v>129</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="143"/>
-      <c r="D1795" s="144"/>
-      <c r="E1795" s="144"/>
+      <c r="C1795" s="147"/>
+      <c r="D1795" s="148"/>
+      <c r="E1795" s="148"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -18993,9 +19461,9 @@
         <v>130</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="143"/>
-      <c r="D1812" s="144"/>
-      <c r="E1812" s="144"/>
+      <c r="C1812" s="147"/>
+      <c r="D1812" s="148"/>
+      <c r="E1812" s="148"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -19146,9 +19614,9 @@
         <v>95</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="143"/>
-      <c r="D1829" s="144"/>
-      <c r="E1829" s="144"/>
+      <c r="C1829" s="147"/>
+      <c r="D1829" s="148"/>
+      <c r="E1829" s="148"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -19299,9 +19767,9 @@
         <v>131</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="143"/>
-      <c r="D1846" s="144"/>
-      <c r="E1846" s="144"/>
+      <c r="C1846" s="147"/>
+      <c r="D1846" s="148"/>
+      <c r="E1846" s="148"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -19452,9 +19920,9 @@
         <v>132</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="143"/>
-      <c r="D1863" s="144"/>
-      <c r="E1863" s="144"/>
+      <c r="C1863" s="147"/>
+      <c r="D1863" s="148"/>
+      <c r="E1863" s="148"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -19605,9 +20073,9 @@
         <v>133</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="143"/>
-      <c r="D1880" s="144"/>
-      <c r="E1880" s="144"/>
+      <c r="C1880" s="147"/>
+      <c r="D1880" s="148"/>
+      <c r="E1880" s="148"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -19758,9 +20226,9 @@
         <v>134</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="143"/>
-      <c r="D1897" s="144"/>
-      <c r="E1897" s="144"/>
+      <c r="C1897" s="147"/>
+      <c r="D1897" s="148"/>
+      <c r="E1897" s="148"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -19911,18 +20379,18 @@
         <v>135</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="147"/>
-      <c r="D1914" s="148"/>
-      <c r="E1914" s="148"/>
+      <c r="C1914" s="151"/>
+      <c r="D1914" s="152"/>
+      <c r="E1914" s="152"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>136</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="143"/>
-      <c r="D1915" s="144"/>
-      <c r="E1915" s="144"/>
+      <c r="C1915" s="147"/>
+      <c r="D1915" s="148"/>
+      <c r="E1915" s="148"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -20073,9 +20541,9 @@
         <v>137</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="145"/>
-      <c r="D1932" s="146"/>
-      <c r="E1932" s="146"/>
+      <c r="C1932" s="149"/>
+      <c r="D1932" s="150"/>
+      <c r="E1932" s="150"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -20226,9 +20694,9 @@
         <v>138</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="143"/>
-      <c r="D1949" s="144"/>
-      <c r="E1949" s="144"/>
+      <c r="C1949" s="147"/>
+      <c r="D1949" s="148"/>
+      <c r="E1949" s="148"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -20379,9 +20847,9 @@
         <v>139</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="143"/>
-      <c r="D1966" s="144"/>
-      <c r="E1966" s="144"/>
+      <c r="C1966" s="147"/>
+      <c r="D1966" s="148"/>
+      <c r="E1966" s="148"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -20532,9 +21000,9 @@
         <v>140</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="143"/>
-      <c r="D1983" s="144"/>
-      <c r="E1983" s="144"/>
+      <c r="C1983" s="147"/>
+      <c r="D1983" s="148"/>
+      <c r="E1983" s="148"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -20685,9 +21153,9 @@
         <v>141</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="143"/>
-      <c r="D2000" s="144"/>
-      <c r="E2000" s="144"/>
+      <c r="C2000" s="147"/>
+      <c r="D2000" s="148"/>
+      <c r="E2000" s="148"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -20838,9 +21306,9 @@
         <v>142</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="143"/>
-      <c r="D2017" s="144"/>
-      <c r="E2017" s="144"/>
+      <c r="C2017" s="147"/>
+      <c r="D2017" s="148"/>
+      <c r="E2017" s="148"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -20991,9 +21459,9 @@
         <v>143</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="143"/>
-      <c r="D2034" s="144"/>
-      <c r="E2034" s="144"/>
+      <c r="C2034" s="147"/>
+      <c r="D2034" s="148"/>
+      <c r="E2034" s="148"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -21144,9 +21612,9 @@
         <v>144</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="143"/>
-      <c r="D2051" s="144"/>
-      <c r="E2051" s="144"/>
+      <c r="C2051" s="147"/>
+      <c r="D2051" s="148"/>
+      <c r="E2051" s="148"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -21297,9 +21765,9 @@
         <v>145</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="143"/>
-      <c r="D2068" s="144"/>
-      <c r="E2068" s="144"/>
+      <c r="C2068" s="147"/>
+      <c r="D2068" s="148"/>
+      <c r="E2068" s="148"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -21450,9 +21918,9 @@
         <v>146</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="143"/>
-      <c r="D2085" s="144"/>
-      <c r="E2085" s="144"/>
+      <c r="C2085" s="147"/>
+      <c r="D2085" s="148"/>
+      <c r="E2085" s="148"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -21603,9 +22071,9 @@
         <v>147</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="143"/>
-      <c r="D2102" s="144"/>
-      <c r="E2102" s="144"/>
+      <c r="C2102" s="147"/>
+      <c r="D2102" s="148"/>
+      <c r="E2102" s="148"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -21756,9 +22224,9 @@
         <v>96</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="143"/>
-      <c r="D2119" s="144"/>
-      <c r="E2119" s="144"/>
+      <c r="C2119" s="147"/>
+      <c r="D2119" s="148"/>
+      <c r="E2119" s="148"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -21909,9 +22377,9 @@
         <v>148</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="143"/>
-      <c r="D2136" s="144"/>
-      <c r="E2136" s="144"/>
+      <c r="C2136" s="147"/>
+      <c r="D2136" s="148"/>
+      <c r="E2136" s="148"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -22062,9 +22530,9 @@
         <v>149</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="143"/>
-      <c r="D2153" s="144"/>
-      <c r="E2153" s="144"/>
+      <c r="C2153" s="147"/>
+      <c r="D2153" s="148"/>
+      <c r="E2153" s="148"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -22215,9 +22683,9 @@
         <v>150</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="143"/>
-      <c r="D2170" s="144"/>
-      <c r="E2170" s="144"/>
+      <c r="C2170" s="147"/>
+      <c r="D2170" s="148"/>
+      <c r="E2170" s="148"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -22503,7 +22971,7 @@
     <mergeCell ref="C2136:E2136"/>
     <mergeCell ref="C2153:E2153"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -22528,51 +22996,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="170" t="s">
+      <c r="A1" s="174" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
+      <c r="H1" s="174"/>
+      <c r="I1" s="174"/>
+      <c r="J1" s="174"/>
+      <c r="K1" s="174"/>
+      <c r="L1" s="174"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="167" t="s">
+      <c r="A2" s="171" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="168"/>
-      <c r="C2" s="168"/>
-      <c r="D2" s="168"/>
-      <c r="E2" s="168"/>
-      <c r="F2" s="168"/>
-      <c r="G2" s="168"/>
-      <c r="H2" s="168"/>
-      <c r="I2" s="168"/>
-      <c r="J2" s="168"/>
-      <c r="K2" s="168"/>
-      <c r="L2" s="169"/>
+      <c r="B2" s="172"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="172"/>
+      <c r="E2" s="172"/>
+      <c r="F2" s="172"/>
+      <c r="G2" s="172"/>
+      <c r="H2" s="172"/>
+      <c r="I2" s="172"/>
+      <c r="J2" s="172"/>
+      <c r="K2" s="172"/>
+      <c r="L2" s="173"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="164" t="s">
+      <c r="A3" s="168" t="s">
         <v>157</v>
       </c>
-      <c r="B3" s="165"/>
-      <c r="C3" s="165"/>
-      <c r="D3" s="165"/>
-      <c r="E3" s="165"/>
-      <c r="F3" s="165"/>
-      <c r="G3" s="165"/>
-      <c r="H3" s="165"/>
-      <c r="I3" s="165"/>
-      <c r="J3" s="165"/>
-      <c r="K3" s="166"/>
+      <c r="B3" s="169"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="169"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="169"/>
+      <c r="K3" s="170"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1">
       <c r="A4" s="28" t="s">
@@ -22789,19 +23257,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A20" s="164" t="s">
+      <c r="A20" s="168" t="s">
         <v>165</v>
       </c>
-      <c r="B20" s="165"/>
-      <c r="C20" s="165"/>
-      <c r="D20" s="165"/>
-      <c r="E20" s="165"/>
-      <c r="F20" s="165"/>
-      <c r="G20" s="165"/>
-      <c r="H20" s="165"/>
-      <c r="I20" s="165"/>
-      <c r="J20" s="165"/>
-      <c r="K20" s="166"/>
+      <c r="B20" s="169"/>
+      <c r="C20" s="169"/>
+      <c r="D20" s="169"/>
+      <c r="E20" s="169"/>
+      <c r="F20" s="169"/>
+      <c r="G20" s="169"/>
+      <c r="H20" s="169"/>
+      <c r="I20" s="169"/>
+      <c r="J20" s="169"/>
+      <c r="K20" s="170"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="28" t="s">
@@ -23018,19 +23486,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A37" s="164" t="s">
+      <c r="A37" s="168" t="s">
         <v>166</v>
       </c>
-      <c r="B37" s="165"/>
-      <c r="C37" s="165"/>
-      <c r="D37" s="165"/>
-      <c r="E37" s="165"/>
-      <c r="F37" s="165"/>
-      <c r="G37" s="165"/>
-      <c r="H37" s="165"/>
-      <c r="I37" s="165"/>
-      <c r="J37" s="165"/>
-      <c r="K37" s="166"/>
+      <c r="B37" s="169"/>
+      <c r="C37" s="169"/>
+      <c r="D37" s="169"/>
+      <c r="E37" s="169"/>
+      <c r="F37" s="169"/>
+      <c r="G37" s="169"/>
+      <c r="H37" s="169"/>
+      <c r="I37" s="169"/>
+      <c r="J37" s="169"/>
+      <c r="K37" s="170"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="28" t="s">
@@ -23254,7 +23722,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -23288,28 +23756,28 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="171"/>
+      <c r="A3" s="175"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="172"/>
+      <c r="A4" s="176"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="172"/>
+      <c r="A5" s="176"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="172"/>
+      <c r="A6" s="176"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="172"/>
+      <c r="A7" s="176"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="172"/>
+      <c r="A8" s="176"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="172"/>
+      <c r="A9" s="176"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1">
-      <c r="A10" s="173"/>
+      <c r="A10" s="177"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1">
       <c r="A11" s="22" t="s">
@@ -23465,7 +23933,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -23488,14 +23956,14 @@
   <cols>
     <col min="1" max="1" width="5.28515625" customWidth="1"/>
     <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="114" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="113" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="174" t="s">
+      <c r="B1" s="178" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="175"/>
+      <c r="C1" s="179"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -23503,16 +23971,16 @@
       <c r="B2" s="94"/>
       <c r="C2" s="94"/>
       <c r="D2" s="92"/>
-      <c r="E2" s="110"/>
+      <c r="E2" s="109"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="176" t="s">
+      <c r="A3" s="180" t="s">
         <v>201</v>
       </c>
-      <c r="B3" s="118" t="s">
+      <c r="B3" s="117" t="s">
         <v>171</v>
       </c>
-      <c r="C3" s="117" t="str">
+      <c r="C3" s="116" t="str">
         <f>FrameCounts!B2</f>
         <v>version</v>
       </c>
@@ -23520,11 +23988,11 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="177"/>
-      <c r="B4" s="115" t="s">
+      <c r="A4" s="181"/>
+      <c r="B4" s="114" t="s">
         <v>158</v>
       </c>
-      <c r="C4" s="119" t="str">
+      <c r="C4" s="118" t="str">
         <f>FrameCounts!B3</f>
         <v>name</v>
       </c>
@@ -23532,20 +24000,20 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="177"/>
-      <c r="B5" s="115" t="s">
+      <c r="A5" s="181"/>
+      <c r="B5" s="114" t="s">
         <v>159</v>
       </c>
-      <c r="C5" s="120"/>
+      <c r="C5" s="119"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="177"/>
-      <c r="B6" s="126" t="s">
+      <c r="A6" s="181"/>
+      <c r="B6" s="125" t="s">
         <v>203</v>
       </c>
-      <c r="C6" s="121">
+      <c r="C6" s="120">
         <f>FrameCounts!H2</f>
         <v>0</v>
       </c>
@@ -23553,11 +24021,11 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="177"/>
-      <c r="B7" s="115" t="s">
+      <c r="A7" s="181"/>
+      <c r="B7" s="114" t="s">
         <v>169</v>
       </c>
-      <c r="C7" s="122">
+      <c r="C7" s="121">
         <f>C6/60</f>
         <v>0</v>
       </c>
@@ -23565,37 +24033,37 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="177"/>
-      <c r="B8" s="115" t="s">
+      <c r="A8" s="181"/>
+      <c r="B8" s="114" t="s">
         <v>170</v>
       </c>
-      <c r="C8" s="119"/>
+      <c r="C8" s="118"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="178"/>
-      <c r="B9" s="123" t="s">
+      <c r="A9" s="182"/>
+      <c r="B9" s="122" t="s">
         <v>160</v>
       </c>
-      <c r="C9" s="124"/>
-      <c r="D9" s="125"/>
+      <c r="C9" s="123"/>
+      <c r="D9" s="124"/>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="13.5" thickBot="1">
-      <c r="B10" s="115"/>
-      <c r="C10" s="116"/>
+      <c r="B10" s="114"/>
+      <c r="C10" s="115"/>
       <c r="D10" s="94"/>
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="180" t="s">
         <v>202</v>
       </c>
-      <c r="B11" s="118" t="s">
+      <c r="B11" s="117" t="s">
         <v>171</v>
       </c>
-      <c r="C11" s="117" t="str">
+      <c r="C11" s="116" t="str">
         <f>FrameCounts!B12</f>
         <v>Knockdown 1</v>
       </c>
@@ -23603,11 +24071,11 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="177"/>
-      <c r="B12" s="115" t="s">
+      <c r="A12" s="181"/>
+      <c r="B12" s="114" t="s">
         <v>158</v>
       </c>
-      <c r="C12" s="119" t="str">
+      <c r="C12" s="118" t="str">
         <f>FrameCounts!B13</f>
         <v>Knockdown 2</v>
       </c>
@@ -23615,20 +24083,20 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="177"/>
-      <c r="B13" s="115" t="s">
+      <c r="A13" s="181"/>
+      <c r="B13" s="114" t="s">
         <v>159</v>
       </c>
-      <c r="C13" s="120"/>
+      <c r="C13" s="119"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="177"/>
-      <c r="B14" s="126" t="s">
+      <c r="A14" s="181"/>
+      <c r="B14" s="125" t="s">
         <v>203</v>
       </c>
-      <c r="C14" s="121">
+      <c r="C14" s="120">
         <f>FrameCounts!H12</f>
         <v>0</v>
       </c>
@@ -23636,11 +24104,11 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="177"/>
-      <c r="B15" s="115" t="s">
+      <c r="A15" s="181"/>
+      <c r="B15" s="114" t="s">
         <v>169</v>
       </c>
-      <c r="C15" s="122">
+      <c r="C15" s="121">
         <f>C14/60</f>
         <v>0</v>
       </c>
@@ -23648,88 +24116,88 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="177"/>
-      <c r="B16" s="115" t="s">
+      <c r="A16" s="181"/>
+      <c r="B16" s="114" t="s">
         <v>170</v>
       </c>
-      <c r="C16" s="119"/>
+      <c r="C16" s="118"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="178"/>
-      <c r="B17" s="123" t="s">
+      <c r="A17" s="182"/>
+      <c r="B17" s="122" t="s">
         <v>160</v>
       </c>
-      <c r="C17" s="124"/>
+      <c r="C17" s="123"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" ht="13.5" thickBot="1">
-      <c r="B18" s="115"/>
-      <c r="C18" s="116"/>
+      <c r="B18" s="114"/>
+      <c r="C18" s="115"/>
       <c r="D18" s="94"/>
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="176" t="s">
+      <c r="A19" s="180" t="s">
         <v>202</v>
       </c>
-      <c r="B19" s="118" t="s">
+      <c r="B19" s="117" t="s">
         <v>171</v>
       </c>
-      <c r="C19" s="117"/>
+      <c r="C19" s="116"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="177"/>
-      <c r="B20" s="115" t="s">
+      <c r="A20" s="181"/>
+      <c r="B20" s="114" t="s">
         <v>158</v>
       </c>
-      <c r="C20" s="119" t="e">
+      <c r="C20" s="118" t="e">
         <f>FrameCounts!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="177"/>
-      <c r="B21" s="115" t="s">
+      <c r="A21" s="181"/>
+      <c r="B21" s="114" t="s">
         <v>159</v>
       </c>
-      <c r="C21" s="120"/>
+      <c r="C21" s="119"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="177"/>
-      <c r="B22" s="126" t="s">
+      <c r="A22" s="181"/>
+      <c r="B22" s="125" t="s">
         <v>203</v>
       </c>
-      <c r="C22" s="121" t="e">
+      <c r="C22" s="120" t="e">
         <f>FrameCounts!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="177"/>
-      <c r="B23" s="115" t="s">
+      <c r="A23" s="181"/>
+      <c r="B23" s="114" t="s">
         <v>169</v>
       </c>
-      <c r="C23" s="122" t="e">
+      <c r="C23" s="121" t="e">
         <f>C22/60</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="177"/>
-      <c r="B24" s="115" t="s">
+      <c r="A24" s="181"/>
+      <c r="B24" s="114" t="s">
         <v>170</v>
       </c>
-      <c r="C24" s="119"/>
+      <c r="C24" s="118"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="178"/>
-      <c r="B25" s="123" t="s">
+      <c r="A25" s="182"/>
+      <c r="B25" s="122" t="s">
         <v>160</v>
       </c>
-      <c r="C25" s="124"/>
+      <c r="C25" s="123"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -23738,7 +24206,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -23760,147 +24228,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="192" t="s">
         <v>183</v>
       </c>
-      <c r="B1" s="189"/>
-      <c r="C1" s="109"/>
+      <c r="B1" s="193"/>
+      <c r="C1" s="108"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="185" t="s">
+      <c r="A2" s="189" t="s">
         <v>182</v>
       </c>
-      <c r="B2" s="186"/>
-      <c r="C2" s="111"/>
+      <c r="B2" s="190"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="187" t="s">
+      <c r="A3" s="191" t="s">
         <v>184</v>
       </c>
-      <c r="B3" s="186"/>
-      <c r="C3" s="111"/>
+      <c r="B3" s="190"/>
+      <c r="C3" s="110"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="192"/>
-      <c r="B4" s="193"/>
-      <c r="C4" s="111"/>
+      <c r="A4" s="196"/>
+      <c r="B4" s="197"/>
+      <c r="C4" s="110"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="190" t="s">
+      <c r="A5" s="194" t="s">
         <v>193</v>
       </c>
-      <c r="B5" s="191"/>
-      <c r="C5" s="111"/>
+      <c r="B5" s="195"/>
+      <c r="C5" s="110"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="196" t="s">
+      <c r="A7" s="200" t="s">
         <v>185</v>
       </c>
-      <c r="B7" s="197"/>
+      <c r="B7" s="201"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="111"/>
+      <c r="A8" s="110"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="194" t="s">
+      <c r="A9" s="198" t="s">
         <v>186</v>
       </c>
-      <c r="B9" s="195"/>
+      <c r="B9" s="199"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="181"/>
-      <c r="B10" s="182"/>
+      <c r="A10" s="185"/>
+      <c r="B10" s="186"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="183" t="s">
+      <c r="A11" s="187" t="s">
         <v>187</v>
       </c>
-      <c r="B11" s="184"/>
+      <c r="B11" s="188"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="183" t="s">
+      <c r="A12" s="187" t="s">
         <v>188</v>
       </c>
-      <c r="B12" s="184"/>
+      <c r="B12" s="188"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="183" t="s">
+      <c r="A13" s="187" t="s">
         <v>189</v>
       </c>
-      <c r="B13" s="184"/>
+      <c r="B13" s="188"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="183" t="s">
+      <c r="A14" s="187" t="s">
         <v>190</v>
       </c>
-      <c r="B14" s="184"/>
+      <c r="B14" s="188"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="183" t="s">
+      <c r="A15" s="187" t="s">
         <v>191</v>
       </c>
-      <c r="B15" s="184"/>
+      <c r="B15" s="188"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="183" t="s">
+      <c r="A16" s="187" t="s">
         <v>192</v>
       </c>
-      <c r="B16" s="184"/>
+      <c r="B16" s="188"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="179" t="s">
+      <c r="A17" s="183" t="s">
         <v>194</v>
       </c>
-      <c r="B17" s="180"/>
+      <c r="B17" s="184"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="196" t="s">
+      <c r="A19" s="200" t="s">
         <v>196</v>
       </c>
-      <c r="B19" s="197"/>
+      <c r="B19" s="201"/>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="111"/>
+      <c r="A20" s="110"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="194" t="s">
+      <c r="A21" s="198" t="s">
         <v>197</v>
       </c>
-      <c r="B21" s="195"/>
+      <c r="B21" s="199"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="181"/>
-      <c r="B22" s="182"/>
+      <c r="A22" s="185"/>
+      <c r="B22" s="186"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="183" t="s">
+      <c r="A23" s="187" t="s">
         <v>198</v>
       </c>
-      <c r="B23" s="184"/>
+      <c r="B23" s="188"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="183"/>
-      <c r="B24" s="184"/>
+      <c r="A24" s="187"/>
+      <c r="B24" s="188"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="183" t="s">
+      <c r="A25" s="187" t="s">
         <v>199</v>
       </c>
-      <c r="B25" s="184"/>
+      <c r="B25" s="188"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="183" t="s">
+      <c r="A26" s="187" t="s">
         <v>200</v>
       </c>
-      <c r="B26" s="184"/>
+      <c r="B26" s="188"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="179"/>
-      <c r="B27" s="180"/>
+      <c r="A27" s="183"/>
+      <c r="B27" s="184"/>
     </row>
   </sheetData>
   <mergeCells count="23">

</xml_diff>

<commit_message>
Pit Fighter - Done
</commit_message>
<xml_diff>
--- a/PitFighter/PitFighter.xlsx
+++ b/PitFighter/PitFighter.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="225">
   <si>
     <t>Notes</t>
   </si>
@@ -729,6 +729,12 @@
   <si>
     <t>Begin Fight 13</t>
   </si>
+  <si>
+    <t>Begin Final Fight</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
 </sst>
 </file>
 
@@ -737,10 +743,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="50">
+  <fonts count="51">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1654,34 +1667,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="203">
+  <cellXfs count="204">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1689,182 +1702,182 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="27" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="29" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="30" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="30" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="30" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="30" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="31" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="31" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="31" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="41" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="32" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="30" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="33" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="31" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1874,10 +1887,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1898,144 +1911,147 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="48" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="49" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="49" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="38" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="48" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="37" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="38" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="33" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -2349,8 +2365,8 @@
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+      <pane ySplit="6" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="1"/>
@@ -2366,16 +2382,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="143" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="141"/>
-      <c r="C1" s="143" t="s">
+      <c r="B1" s="142"/>
+      <c r="C1" s="144" t="s">
         <v>168</v>
       </c>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="145"/>
       <c r="G1" s="126"/>
       <c r="H1" s="127">
         <f>SUM(G1:G65351)</f>
@@ -2453,10 +2469,10 @@
       <c r="B5" s="133" t="s">
         <v>175</v>
       </c>
-      <c r="C5" s="140" t="s">
+      <c r="C5" s="141" t="s">
         <v>177</v>
       </c>
-      <c r="D5" s="140"/>
+      <c r="D5" s="141"/>
       <c r="E5" s="133"/>
       <c r="F5" s="129"/>
       <c r="G5" s="126"/>
@@ -2472,10 +2488,10 @@
       <c r="B6" s="133" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="140" t="s">
+      <c r="C6" s="141" t="s">
         <v>167</v>
       </c>
-      <c r="D6" s="141"/>
+      <c r="D6" s="142"/>
       <c r="E6" s="133"/>
       <c r="F6" s="129"/>
       <c r="G6" s="126"/>
@@ -2493,7 +2509,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="145" t="s">
+      <c r="A8" s="146" t="s">
         <v>204</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2513,7 +2529,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A9" s="146"/>
+      <c r="A9" s="147"/>
       <c r="B9" s="98" t="s">
         <v>175</v>
       </c>
@@ -2523,7 +2539,7 @@
       <c r="F9" s="103"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A10" s="146"/>
+      <c r="A10" s="147"/>
       <c r="B10" s="134" t="s">
         <v>206</v>
       </c>
@@ -2540,7 +2556,7 @@
       <c r="F10" s="104"/>
     </row>
     <row r="11" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A11" s="146"/>
+      <c r="A11" s="147"/>
       <c r="B11" s="134" t="s">
         <v>211</v>
       </c>
@@ -2557,7 +2573,7 @@
       <c r="F11" s="104"/>
     </row>
     <row r="12" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A12" s="146"/>
+      <c r="A12" s="147"/>
       <c r="B12" s="134" t="s">
         <v>208</v>
       </c>
@@ -2574,7 +2590,7 @@
       <c r="F12" s="104"/>
     </row>
     <row r="13" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A13" s="146"/>
+      <c r="A13" s="147"/>
       <c r="B13" s="134" t="s">
         <v>209</v>
       </c>
@@ -2589,7 +2605,7 @@
       <c r="F13" s="104"/>
     </row>
     <row r="14" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A14" s="146"/>
+      <c r="A14" s="147"/>
       <c r="B14" s="134" t="s">
         <v>210</v>
       </c>
@@ -2606,7 +2622,7 @@
       <c r="F14" s="104"/>
     </row>
     <row r="15" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A15" s="146"/>
+      <c r="A15" s="147"/>
       <c r="B15" s="135" t="s">
         <v>212</v>
       </c>
@@ -2623,7 +2639,7 @@
       <c r="F15" s="104"/>
     </row>
     <row r="16" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A16" s="146"/>
+      <c r="A16" s="147"/>
       <c r="B16" s="134" t="s">
         <v>208</v>
       </c>
@@ -2640,7 +2656,7 @@
       <c r="F16" s="104"/>
     </row>
     <row r="17" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A17" s="146"/>
+      <c r="A17" s="147"/>
       <c r="B17" s="134" t="s">
         <v>209</v>
       </c>
@@ -2657,7 +2673,7 @@
       <c r="F17" s="104"/>
     </row>
     <row r="18" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A18" s="146"/>
+      <c r="A18" s="147"/>
       <c r="B18" s="134" t="s">
         <v>210</v>
       </c>
@@ -2674,7 +2690,7 @@
       <c r="F18" s="104"/>
     </row>
     <row r="19" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A19" s="146"/>
+      <c r="A19" s="147"/>
       <c r="B19" s="136" t="s">
         <v>213</v>
       </c>
@@ -2691,7 +2707,7 @@
       <c r="F19" s="104"/>
     </row>
     <row r="20" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A20" s="146"/>
+      <c r="A20" s="147"/>
       <c r="B20" s="136" t="s">
         <v>214</v>
       </c>
@@ -2708,7 +2724,7 @@
       <c r="F20" s="104"/>
     </row>
     <row r="21" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A21" s="146"/>
+      <c r="A21" s="147"/>
       <c r="B21" s="138" t="s">
         <v>215</v>
       </c>
@@ -2725,7 +2741,7 @@
       <c r="F21" s="104"/>
     </row>
     <row r="22" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A22" s="146"/>
+      <c r="A22" s="147"/>
       <c r="B22" s="139" t="s">
         <v>216</v>
       </c>
@@ -2742,7 +2758,7 @@
       <c r="F22" s="104"/>
     </row>
     <row r="23" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A23" s="146"/>
+      <c r="A23" s="147"/>
       <c r="B23" s="139" t="s">
         <v>208</v>
       </c>
@@ -2759,7 +2775,7 @@
       <c r="F23" s="104"/>
     </row>
     <row r="24" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A24" s="146"/>
+      <c r="A24" s="147"/>
       <c r="B24" s="139" t="s">
         <v>209</v>
       </c>
@@ -2776,7 +2792,7 @@
       <c r="F24" s="104"/>
     </row>
     <row r="25" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A25" s="146"/>
+      <c r="A25" s="147"/>
       <c r="B25" s="139" t="s">
         <v>210</v>
       </c>
@@ -2793,7 +2809,7 @@
       <c r="F25" s="104"/>
     </row>
     <row r="26" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A26" s="146"/>
+      <c r="A26" s="147"/>
       <c r="B26" s="139" t="s">
         <v>213</v>
       </c>
@@ -2810,8 +2826,8 @@
       <c r="F26" s="104"/>
     </row>
     <row r="27" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A27" s="146"/>
-      <c r="B27" s="202" t="s">
+      <c r="A27" s="147"/>
+      <c r="B27" s="140" t="s">
         <v>217</v>
       </c>
       <c r="C27" s="100">
@@ -2827,8 +2843,8 @@
       <c r="F27" s="104"/>
     </row>
     <row r="28" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A28" s="146"/>
-      <c r="B28" s="202" t="s">
+      <c r="A28" s="147"/>
+      <c r="B28" s="140" t="s">
         <v>213</v>
       </c>
       <c r="C28" s="100">
@@ -2844,8 +2860,8 @@
       <c r="F28" s="104"/>
     </row>
     <row r="29" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A29" s="146"/>
-      <c r="B29" s="202" t="s">
+      <c r="A29" s="147"/>
+      <c r="B29" s="140" t="s">
         <v>218</v>
       </c>
       <c r="C29" s="100">
@@ -2861,8 +2877,8 @@
       <c r="F29" s="104"/>
     </row>
     <row r="30" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A30" s="146"/>
-      <c r="B30" s="202" t="s">
+      <c r="A30" s="147"/>
+      <c r="B30" s="140" t="s">
         <v>213</v>
       </c>
       <c r="C30" s="100">
@@ -2878,8 +2894,8 @@
       <c r="F30" s="104"/>
     </row>
     <row r="31" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A31" s="146"/>
-      <c r="B31" s="202" t="s">
+      <c r="A31" s="147"/>
+      <c r="B31" s="140" t="s">
         <v>219</v>
       </c>
       <c r="C31" s="100">
@@ -2895,7 +2911,7 @@
       <c r="F31" s="104"/>
     </row>
     <row r="32" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A32" s="146"/>
+      <c r="A32" s="147"/>
       <c r="B32" s="134" t="s">
         <v>208</v>
       </c>
@@ -2912,7 +2928,7 @@
       <c r="F32" s="104"/>
     </row>
     <row r="33" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A33" s="146"/>
+      <c r="A33" s="147"/>
       <c r="B33" s="134" t="s">
         <v>209</v>
       </c>
@@ -2929,7 +2945,7 @@
       <c r="F33" s="104"/>
     </row>
     <row r="34" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A34" s="146"/>
+      <c r="A34" s="147"/>
       <c r="B34" s="134" t="s">
         <v>210</v>
       </c>
@@ -2946,8 +2962,8 @@
       <c r="F34" s="104"/>
     </row>
     <row r="35" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A35" s="146"/>
-      <c r="B35" s="202" t="s">
+      <c r="A35" s="147"/>
+      <c r="B35" s="140" t="s">
         <v>220</v>
       </c>
       <c r="C35" s="100">
@@ -2963,8 +2979,8 @@
       <c r="F35" s="104"/>
     </row>
     <row r="36" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A36" s="146"/>
-      <c r="B36" s="202" t="s">
+      <c r="A36" s="147"/>
+      <c r="B36" s="140" t="s">
         <v>222</v>
       </c>
       <c r="C36" s="100">
@@ -2980,8 +2996,8 @@
       <c r="F36" s="104"/>
     </row>
     <row r="37" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A37" s="146"/>
-      <c r="B37" s="202" t="s">
+      <c r="A37" s="147"/>
+      <c r="B37" s="140" t="s">
         <v>220</v>
       </c>
       <c r="C37" s="100">
@@ -2997,8 +3013,8 @@
       <c r="F37" s="104"/>
     </row>
     <row r="38" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A38" s="146"/>
-      <c r="B38" s="202" t="s">
+      <c r="A38" s="147"/>
+      <c r="B38" s="140" t="s">
         <v>221</v>
       </c>
       <c r="C38" s="100">
@@ -3014,26 +3030,30 @@
       <c r="F38" s="104"/>
     </row>
     <row r="39" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A39" s="146"/>
-      <c r="B39" s="202" t="s">
+      <c r="A39" s="147"/>
+      <c r="B39" s="140" t="s">
         <v>220</v>
       </c>
       <c r="C39" s="100">
-        <v>16658</v>
+        <v>16065</v>
       </c>
       <c r="D39" s="100">
         <v>21722</v>
       </c>
       <c r="E39" s="100">
         <f t="shared" si="0"/>
-        <v>5064</v>
+        <v>5657</v>
       </c>
       <c r="F39" s="104"/>
     </row>
     <row r="40" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A40" s="146"/>
-      <c r="B40" s="202"/>
-      <c r="C40" s="100"/>
+      <c r="A40" s="147"/>
+      <c r="B40" s="140" t="s">
+        <v>223</v>
+      </c>
+      <c r="C40" s="100">
+        <v>16691</v>
+      </c>
       <c r="D40" s="100"/>
       <c r="E40" s="100">
         <f t="shared" si="0"/>
@@ -3042,18 +3062,24 @@
       <c r="F40" s="104"/>
     </row>
     <row r="41" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A41" s="146"/>
-      <c r="B41" s="134"/>
-      <c r="C41" s="100"/>
-      <c r="D41" s="100"/>
+      <c r="A41" s="147"/>
+      <c r="B41" s="203" t="s">
+        <v>224</v>
+      </c>
+      <c r="C41" s="100">
+        <v>17293</v>
+      </c>
+      <c r="D41" s="100">
+        <v>23432</v>
+      </c>
       <c r="E41" s="100">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6139</v>
       </c>
       <c r="F41" s="104"/>
     </row>
     <row r="42" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A42" s="146"/>
+      <c r="A42" s="147"/>
       <c r="B42" s="134"/>
       <c r="C42" s="100"/>
       <c r="D42" s="100"/>
@@ -3064,7 +3090,7 @@
       <c r="F42" s="104"/>
     </row>
     <row r="43" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A43" s="146"/>
+      <c r="A43" s="147"/>
       <c r="B43" s="98" t="s">
         <v>178</v>
       </c>
@@ -3143,13 +3169,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="148" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="165"/>
-      <c r="C1" s="165"/>
-      <c r="D1" s="165"/>
-      <c r="E1" s="165"/>
+      <c r="B1" s="148"/>
+      <c r="C1" s="148"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -3179,18 +3205,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="167"/>
-      <c r="E3" s="167"/>
+      <c r="C3" s="149"/>
+      <c r="D3" s="150"/>
+      <c r="E3" s="150"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="147"/>
-      <c r="D4" s="148"/>
-      <c r="E4" s="148"/>
+      <c r="C4" s="151"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="152"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -3342,9 +3368,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="149"/>
-      <c r="D21" s="150"/>
-      <c r="E21" s="150"/>
+      <c r="C21" s="153"/>
+      <c r="D21" s="154"/>
+      <c r="E21" s="154"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -3495,9 +3521,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="147"/>
-      <c r="D38" s="148"/>
-      <c r="E38" s="148"/>
+      <c r="C38" s="151"/>
+      <c r="D38" s="152"/>
+      <c r="E38" s="152"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -3648,9 +3674,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="147"/>
-      <c r="D55" s="148"/>
-      <c r="E55" s="148"/>
+      <c r="C55" s="151"/>
+      <c r="D55" s="152"/>
+      <c r="E55" s="152"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -3801,9 +3827,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="147"/>
-      <c r="D72" s="148"/>
-      <c r="E72" s="148"/>
+      <c r="C72" s="151"/>
+      <c r="D72" s="152"/>
+      <c r="E72" s="152"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -3954,9 +3980,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="147"/>
-      <c r="D89" s="148"/>
-      <c r="E89" s="148"/>
+      <c r="C89" s="151"/>
+      <c r="D89" s="152"/>
+      <c r="E89" s="152"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -4107,9 +4133,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="147"/>
-      <c r="D106" s="148"/>
-      <c r="E106" s="148"/>
+      <c r="C106" s="151"/>
+      <c r="D106" s="152"/>
+      <c r="E106" s="152"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -4260,9 +4286,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="147"/>
-      <c r="D123" s="148"/>
-      <c r="E123" s="148"/>
+      <c r="C123" s="151"/>
+      <c r="D123" s="152"/>
+      <c r="E123" s="152"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -4413,9 +4439,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="147"/>
-      <c r="D140" s="148"/>
-      <c r="E140" s="148"/>
+      <c r="C140" s="151"/>
+      <c r="D140" s="152"/>
+      <c r="E140" s="152"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -4566,9 +4592,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="147"/>
-      <c r="D157" s="148"/>
-      <c r="E157" s="148"/>
+      <c r="C157" s="151"/>
+      <c r="D157" s="152"/>
+      <c r="E157" s="152"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -4719,9 +4745,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="147"/>
-      <c r="D174" s="148"/>
-      <c r="E174" s="148"/>
+      <c r="C174" s="151"/>
+      <c r="D174" s="152"/>
+      <c r="E174" s="152"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -4872,9 +4898,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="147"/>
-      <c r="D191" s="148"/>
-      <c r="E191" s="148"/>
+      <c r="C191" s="151"/>
+      <c r="D191" s="152"/>
+      <c r="E191" s="152"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -5025,9 +5051,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="147"/>
-      <c r="D208" s="148"/>
-      <c r="E208" s="148"/>
+      <c r="C208" s="151"/>
+      <c r="D208" s="152"/>
+      <c r="E208" s="152"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -5178,9 +5204,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="147"/>
-      <c r="D225" s="148"/>
-      <c r="E225" s="148"/>
+      <c r="C225" s="151"/>
+      <c r="D225" s="152"/>
+      <c r="E225" s="152"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -5331,9 +5357,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="147"/>
-      <c r="D242" s="148"/>
-      <c r="E242" s="148"/>
+      <c r="C242" s="151"/>
+      <c r="D242" s="152"/>
+      <c r="E242" s="152"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -5484,9 +5510,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="147"/>
-      <c r="D259" s="148"/>
-      <c r="E259" s="148"/>
+      <c r="C259" s="151"/>
+      <c r="D259" s="152"/>
+      <c r="E259" s="152"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -5637,18 +5663,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="163"/>
-      <c r="D276" s="164"/>
-      <c r="E276" s="164"/>
+      <c r="C276" s="155"/>
+      <c r="D276" s="156"/>
+      <c r="E276" s="156"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="147"/>
-      <c r="D277" s="148"/>
-      <c r="E277" s="148"/>
+      <c r="C277" s="151"/>
+      <c r="D277" s="152"/>
+      <c r="E277" s="152"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -5799,9 +5825,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="149"/>
-      <c r="D294" s="150"/>
-      <c r="E294" s="150"/>
+      <c r="C294" s="153"/>
+      <c r="D294" s="154"/>
+      <c r="E294" s="154"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -5952,9 +5978,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="147"/>
-      <c r="D311" s="148"/>
-      <c r="E311" s="148"/>
+      <c r="C311" s="151"/>
+      <c r="D311" s="152"/>
+      <c r="E311" s="152"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -6105,9 +6131,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="147"/>
-      <c r="D328" s="148"/>
-      <c r="E328" s="148"/>
+      <c r="C328" s="151"/>
+      <c r="D328" s="152"/>
+      <c r="E328" s="152"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -6258,9 +6284,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="147"/>
-      <c r="D345" s="148"/>
-      <c r="E345" s="148"/>
+      <c r="C345" s="151"/>
+      <c r="D345" s="152"/>
+      <c r="E345" s="152"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -6411,9 +6437,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="147"/>
-      <c r="D362" s="148"/>
-      <c r="E362" s="148"/>
+      <c r="C362" s="151"/>
+      <c r="D362" s="152"/>
+      <c r="E362" s="152"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -6564,9 +6590,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="147"/>
-      <c r="D379" s="148"/>
-      <c r="E379" s="148"/>
+      <c r="C379" s="151"/>
+      <c r="D379" s="152"/>
+      <c r="E379" s="152"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -6717,9 +6743,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="147"/>
-      <c r="D396" s="148"/>
-      <c r="E396" s="148"/>
+      <c r="C396" s="151"/>
+      <c r="D396" s="152"/>
+      <c r="E396" s="152"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -6870,9 +6896,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="147"/>
-      <c r="D413" s="148"/>
-      <c r="E413" s="148"/>
+      <c r="C413" s="151"/>
+      <c r="D413" s="152"/>
+      <c r="E413" s="152"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -7023,9 +7049,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="147"/>
-      <c r="D430" s="148"/>
-      <c r="E430" s="148"/>
+      <c r="C430" s="151"/>
+      <c r="D430" s="152"/>
+      <c r="E430" s="152"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -7176,9 +7202,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="147"/>
-      <c r="D447" s="148"/>
-      <c r="E447" s="148"/>
+      <c r="C447" s="151"/>
+      <c r="D447" s="152"/>
+      <c r="E447" s="152"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -7329,9 +7355,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="147"/>
-      <c r="D464" s="148"/>
-      <c r="E464" s="148"/>
+      <c r="C464" s="151"/>
+      <c r="D464" s="152"/>
+      <c r="E464" s="152"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -7482,9 +7508,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="147"/>
-      <c r="D481" s="148"/>
-      <c r="E481" s="148"/>
+      <c r="C481" s="151"/>
+      <c r="D481" s="152"/>
+      <c r="E481" s="152"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -7635,9 +7661,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="147"/>
-      <c r="D498" s="148"/>
-      <c r="E498" s="148"/>
+      <c r="C498" s="151"/>
+      <c r="D498" s="152"/>
+      <c r="E498" s="152"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -7788,9 +7814,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="147"/>
-      <c r="D515" s="148"/>
-      <c r="E515" s="148"/>
+      <c r="C515" s="151"/>
+      <c r="D515" s="152"/>
+      <c r="E515" s="152"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -7941,9 +7967,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="147"/>
-      <c r="D532" s="148"/>
-      <c r="E532" s="148"/>
+      <c r="C532" s="151"/>
+      <c r="D532" s="152"/>
+      <c r="E532" s="152"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -8094,18 +8120,18 @@
         <v>49</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="161"/>
-      <c r="D549" s="162"/>
-      <c r="E549" s="162"/>
+      <c r="C549" s="157"/>
+      <c r="D549" s="158"/>
+      <c r="E549" s="158"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>50</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="147"/>
-      <c r="D550" s="148"/>
-      <c r="E550" s="148"/>
+      <c r="C550" s="151"/>
+      <c r="D550" s="152"/>
+      <c r="E550" s="152"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -8256,9 +8282,9 @@
         <v>51</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="149"/>
-      <c r="D567" s="150"/>
-      <c r="E567" s="150"/>
+      <c r="C567" s="153"/>
+      <c r="D567" s="154"/>
+      <c r="E567" s="154"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -8409,9 +8435,9 @@
         <v>52</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="147"/>
-      <c r="D584" s="148"/>
-      <c r="E584" s="148"/>
+      <c r="C584" s="151"/>
+      <c r="D584" s="152"/>
+      <c r="E584" s="152"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -8562,9 +8588,9 @@
         <v>53</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="147"/>
-      <c r="D601" s="148"/>
-      <c r="E601" s="148"/>
+      <c r="C601" s="151"/>
+      <c r="D601" s="152"/>
+      <c r="E601" s="152"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -8715,9 +8741,9 @@
         <v>54</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="147"/>
-      <c r="D618" s="148"/>
-      <c r="E618" s="148"/>
+      <c r="C618" s="151"/>
+      <c r="D618" s="152"/>
+      <c r="E618" s="152"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -8868,9 +8894,9 @@
         <v>55</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="147"/>
-      <c r="D635" s="148"/>
-      <c r="E635" s="148"/>
+      <c r="C635" s="151"/>
+      <c r="D635" s="152"/>
+      <c r="E635" s="152"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -9021,9 +9047,9 @@
         <v>56</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="147"/>
-      <c r="D652" s="148"/>
-      <c r="E652" s="148"/>
+      <c r="C652" s="151"/>
+      <c r="D652" s="152"/>
+      <c r="E652" s="152"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -9174,9 +9200,9 @@
         <v>57</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="147"/>
-      <c r="D669" s="148"/>
-      <c r="E669" s="148"/>
+      <c r="C669" s="151"/>
+      <c r="D669" s="152"/>
+      <c r="E669" s="152"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -9327,9 +9353,9 @@
         <v>58</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="147"/>
-      <c r="D686" s="148"/>
-      <c r="E686" s="148"/>
+      <c r="C686" s="151"/>
+      <c r="D686" s="152"/>
+      <c r="E686" s="152"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -9480,9 +9506,9 @@
         <v>59</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="147"/>
-      <c r="D703" s="148"/>
-      <c r="E703" s="148"/>
+      <c r="C703" s="151"/>
+      <c r="D703" s="152"/>
+      <c r="E703" s="152"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -9633,9 +9659,9 @@
         <v>60</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="147"/>
-      <c r="D720" s="148"/>
-      <c r="E720" s="148"/>
+      <c r="C720" s="151"/>
+      <c r="D720" s="152"/>
+      <c r="E720" s="152"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -9786,9 +9812,9 @@
         <v>61</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="147"/>
-      <c r="D737" s="148"/>
-      <c r="E737" s="148"/>
+      <c r="C737" s="151"/>
+      <c r="D737" s="152"/>
+      <c r="E737" s="152"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -9939,9 +9965,9 @@
         <v>62</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="147"/>
-      <c r="D754" s="148"/>
-      <c r="E754" s="148"/>
+      <c r="C754" s="151"/>
+      <c r="D754" s="152"/>
+      <c r="E754" s="152"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -10092,9 +10118,9 @@
         <v>63</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="147"/>
-      <c r="D771" s="148"/>
-      <c r="E771" s="148"/>
+      <c r="C771" s="151"/>
+      <c r="D771" s="152"/>
+      <c r="E771" s="152"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -10245,9 +10271,9 @@
         <v>64</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="147"/>
-      <c r="D788" s="148"/>
-      <c r="E788" s="148"/>
+      <c r="C788" s="151"/>
+      <c r="D788" s="152"/>
+      <c r="E788" s="152"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -10398,9 +10424,9 @@
         <v>65</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="147"/>
-      <c r="D805" s="148"/>
-      <c r="E805" s="148"/>
+      <c r="C805" s="151"/>
+      <c r="D805" s="152"/>
+      <c r="E805" s="152"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -10560,9 +10586,9 @@
         <v>67</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="147"/>
-      <c r="D823" s="148"/>
-      <c r="E823" s="148"/>
+      <c r="C823" s="151"/>
+      <c r="D823" s="152"/>
+      <c r="E823" s="152"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -10713,9 +10739,9 @@
         <v>68</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="149"/>
-      <c r="D840" s="150"/>
-      <c r="E840" s="150"/>
+      <c r="C840" s="153"/>
+      <c r="D840" s="154"/>
+      <c r="E840" s="154"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -10866,9 +10892,9 @@
         <v>69</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="147"/>
-      <c r="D857" s="148"/>
-      <c r="E857" s="148"/>
+      <c r="C857" s="151"/>
+      <c r="D857" s="152"/>
+      <c r="E857" s="152"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -11019,9 +11045,9 @@
         <v>70</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="147"/>
-      <c r="D874" s="148"/>
-      <c r="E874" s="148"/>
+      <c r="C874" s="151"/>
+      <c r="D874" s="152"/>
+      <c r="E874" s="152"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -11172,9 +11198,9 @@
         <v>71</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="147"/>
-      <c r="D891" s="148"/>
-      <c r="E891" s="148"/>
+      <c r="C891" s="151"/>
+      <c r="D891" s="152"/>
+      <c r="E891" s="152"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -11325,9 +11351,9 @@
         <v>72</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="147"/>
-      <c r="D908" s="148"/>
-      <c r="E908" s="148"/>
+      <c r="C908" s="151"/>
+      <c r="D908" s="152"/>
+      <c r="E908" s="152"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -11478,9 +11504,9 @@
         <v>73</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="147"/>
-      <c r="D925" s="148"/>
-      <c r="E925" s="148"/>
+      <c r="C925" s="151"/>
+      <c r="D925" s="152"/>
+      <c r="E925" s="152"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -11631,9 +11657,9 @@
         <v>74</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="147"/>
-      <c r="D942" s="148"/>
-      <c r="E942" s="148"/>
+      <c r="C942" s="151"/>
+      <c r="D942" s="152"/>
+      <c r="E942" s="152"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -11784,9 +11810,9 @@
         <v>75</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="147"/>
-      <c r="D959" s="148"/>
-      <c r="E959" s="148"/>
+      <c r="C959" s="151"/>
+      <c r="D959" s="152"/>
+      <c r="E959" s="152"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -11937,9 +11963,9 @@
         <v>76</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="147"/>
-      <c r="D976" s="148"/>
-      <c r="E976" s="148"/>
+      <c r="C976" s="151"/>
+      <c r="D976" s="152"/>
+      <c r="E976" s="152"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -12090,9 +12116,9 @@
         <v>77</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="147"/>
-      <c r="D993" s="148"/>
-      <c r="E993" s="148"/>
+      <c r="C993" s="151"/>
+      <c r="D993" s="152"/>
+      <c r="E993" s="152"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -12243,9 +12269,9 @@
         <v>78</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="147"/>
-      <c r="D1010" s="148"/>
-      <c r="E1010" s="148"/>
+      <c r="C1010" s="151"/>
+      <c r="D1010" s="152"/>
+      <c r="E1010" s="152"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -12396,9 +12422,9 @@
         <v>79</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="147"/>
-      <c r="D1027" s="148"/>
-      <c r="E1027" s="148"/>
+      <c r="C1027" s="151"/>
+      <c r="D1027" s="152"/>
+      <c r="E1027" s="152"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -12549,9 +12575,9 @@
         <v>82</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="147"/>
-      <c r="D1044" s="148"/>
-      <c r="E1044" s="148"/>
+      <c r="C1044" s="151"/>
+      <c r="D1044" s="152"/>
+      <c r="E1044" s="152"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -12702,9 +12728,9 @@
         <v>81</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="147"/>
-      <c r="D1061" s="148"/>
-      <c r="E1061" s="148"/>
+      <c r="C1061" s="151"/>
+      <c r="D1061" s="152"/>
+      <c r="E1061" s="152"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -12855,9 +12881,9 @@
         <v>83</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="147"/>
-      <c r="D1078" s="148"/>
-      <c r="E1078" s="148"/>
+      <c r="C1078" s="151"/>
+      <c r="D1078" s="152"/>
+      <c r="E1078" s="152"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -13008,18 +13034,18 @@
         <v>103</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="157"/>
-      <c r="D1095" s="158"/>
-      <c r="E1095" s="158"/>
+      <c r="C1095" s="161"/>
+      <c r="D1095" s="162"/>
+      <c r="E1095" s="162"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>84</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="147"/>
-      <c r="D1096" s="148"/>
-      <c r="E1096" s="148"/>
+      <c r="C1096" s="151"/>
+      <c r="D1096" s="152"/>
+      <c r="E1096" s="152"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -13170,9 +13196,9 @@
         <v>85</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="149"/>
-      <c r="D1113" s="150"/>
-      <c r="E1113" s="150"/>
+      <c r="C1113" s="153"/>
+      <c r="D1113" s="154"/>
+      <c r="E1113" s="154"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -13323,9 +13349,9 @@
         <v>86</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="147"/>
-      <c r="D1130" s="148"/>
-      <c r="E1130" s="148"/>
+      <c r="C1130" s="151"/>
+      <c r="D1130" s="152"/>
+      <c r="E1130" s="152"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -13476,9 +13502,9 @@
         <v>87</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="147"/>
-      <c r="D1147" s="148"/>
-      <c r="E1147" s="148"/>
+      <c r="C1147" s="151"/>
+      <c r="D1147" s="152"/>
+      <c r="E1147" s="152"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -13629,9 +13655,9 @@
         <v>88</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="147"/>
-      <c r="D1164" s="148"/>
-      <c r="E1164" s="148"/>
+      <c r="C1164" s="151"/>
+      <c r="D1164" s="152"/>
+      <c r="E1164" s="152"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -13782,9 +13808,9 @@
         <v>89</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="147"/>
-      <c r="D1181" s="148"/>
-      <c r="E1181" s="148"/>
+      <c r="C1181" s="151"/>
+      <c r="D1181" s="152"/>
+      <c r="E1181" s="152"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -13935,9 +13961,9 @@
         <v>90</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="147"/>
-      <c r="D1198" s="148"/>
-      <c r="E1198" s="148"/>
+      <c r="C1198" s="151"/>
+      <c r="D1198" s="152"/>
+      <c r="E1198" s="152"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -14088,9 +14114,9 @@
         <v>91</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="147"/>
-      <c r="D1215" s="148"/>
-      <c r="E1215" s="148"/>
+      <c r="C1215" s="151"/>
+      <c r="D1215" s="152"/>
+      <c r="E1215" s="152"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -14241,9 +14267,9 @@
         <v>92</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="147"/>
-      <c r="D1232" s="148"/>
-      <c r="E1232" s="148"/>
+      <c r="C1232" s="151"/>
+      <c r="D1232" s="152"/>
+      <c r="E1232" s="152"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -14394,9 +14420,9 @@
         <v>93</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="147"/>
-      <c r="D1249" s="148"/>
-      <c r="E1249" s="148"/>
+      <c r="C1249" s="151"/>
+      <c r="D1249" s="152"/>
+      <c r="E1249" s="152"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -14547,9 +14573,9 @@
         <v>98</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="147"/>
-      <c r="D1266" s="148"/>
-      <c r="E1266" s="148"/>
+      <c r="C1266" s="151"/>
+      <c r="D1266" s="152"/>
+      <c r="E1266" s="152"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -14700,9 +14726,9 @@
         <v>99</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="147"/>
-      <c r="D1283" s="148"/>
-      <c r="E1283" s="148"/>
+      <c r="C1283" s="151"/>
+      <c r="D1283" s="152"/>
+      <c r="E1283" s="152"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -14853,9 +14879,9 @@
         <v>100</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="147"/>
-      <c r="D1300" s="148"/>
-      <c r="E1300" s="148"/>
+      <c r="C1300" s="151"/>
+      <c r="D1300" s="152"/>
+      <c r="E1300" s="152"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -15006,9 +15032,9 @@
         <v>80</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="147"/>
-      <c r="D1317" s="148"/>
-      <c r="E1317" s="148"/>
+      <c r="C1317" s="151"/>
+      <c r="D1317" s="152"/>
+      <c r="E1317" s="152"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -15159,9 +15185,9 @@
         <v>101</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="147"/>
-      <c r="D1334" s="148"/>
-      <c r="E1334" s="148"/>
+      <c r="C1334" s="151"/>
+      <c r="D1334" s="152"/>
+      <c r="E1334" s="152"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -15312,9 +15338,9 @@
         <v>97</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="147"/>
-      <c r="D1351" s="148"/>
-      <c r="E1351" s="148"/>
+      <c r="C1351" s="151"/>
+      <c r="D1351" s="152"/>
+      <c r="E1351" s="152"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -15465,18 +15491,18 @@
         <v>102</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="155"/>
-      <c r="D1368" s="156"/>
-      <c r="E1368" s="156"/>
+      <c r="C1368" s="163"/>
+      <c r="D1368" s="164"/>
+      <c r="E1368" s="164"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>104</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="147"/>
-      <c r="D1369" s="148"/>
-      <c r="E1369" s="148"/>
+      <c r="C1369" s="151"/>
+      <c r="D1369" s="152"/>
+      <c r="E1369" s="152"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -15627,9 +15653,9 @@
         <v>105</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="149"/>
-      <c r="D1386" s="150"/>
-      <c r="E1386" s="150"/>
+      <c r="C1386" s="153"/>
+      <c r="D1386" s="154"/>
+      <c r="E1386" s="154"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -15780,9 +15806,9 @@
         <v>106</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="147"/>
-      <c r="D1403" s="148"/>
-      <c r="E1403" s="148"/>
+      <c r="C1403" s="151"/>
+      <c r="D1403" s="152"/>
+      <c r="E1403" s="152"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -15933,9 +15959,9 @@
         <v>107</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="147"/>
-      <c r="D1420" s="148"/>
-      <c r="E1420" s="148"/>
+      <c r="C1420" s="151"/>
+      <c r="D1420" s="152"/>
+      <c r="E1420" s="152"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -16086,9 +16112,9 @@
         <v>108</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="147"/>
-      <c r="D1437" s="148"/>
-      <c r="E1437" s="148"/>
+      <c r="C1437" s="151"/>
+      <c r="D1437" s="152"/>
+      <c r="E1437" s="152"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -16239,9 +16265,9 @@
         <v>109</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="147"/>
-      <c r="D1454" s="148"/>
-      <c r="E1454" s="148"/>
+      <c r="C1454" s="151"/>
+      <c r="D1454" s="152"/>
+      <c r="E1454" s="152"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -16392,9 +16418,9 @@
         <v>110</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="147"/>
-      <c r="D1471" s="148"/>
-      <c r="E1471" s="148"/>
+      <c r="C1471" s="151"/>
+      <c r="D1471" s="152"/>
+      <c r="E1471" s="152"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -16545,9 +16571,9 @@
         <v>111</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="147"/>
-      <c r="D1488" s="148"/>
-      <c r="E1488" s="148"/>
+      <c r="C1488" s="151"/>
+      <c r="D1488" s="152"/>
+      <c r="E1488" s="152"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -16698,9 +16724,9 @@
         <v>112</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="147"/>
-      <c r="D1505" s="148"/>
-      <c r="E1505" s="148"/>
+      <c r="C1505" s="151"/>
+      <c r="D1505" s="152"/>
+      <c r="E1505" s="152"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -16851,9 +16877,9 @@
         <v>113</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="147"/>
-      <c r="D1522" s="148"/>
-      <c r="E1522" s="148"/>
+      <c r="C1522" s="151"/>
+      <c r="D1522" s="152"/>
+      <c r="E1522" s="152"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -17004,9 +17030,9 @@
         <v>94</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="147"/>
-      <c r="D1539" s="148"/>
-      <c r="E1539" s="148"/>
+      <c r="C1539" s="151"/>
+      <c r="D1539" s="152"/>
+      <c r="E1539" s="152"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -17157,9 +17183,9 @@
         <v>114</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="147"/>
-      <c r="D1556" s="148"/>
-      <c r="E1556" s="148"/>
+      <c r="C1556" s="151"/>
+      <c r="D1556" s="152"/>
+      <c r="E1556" s="152"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -17310,9 +17336,9 @@
         <v>115</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="147"/>
-      <c r="D1573" s="148"/>
-      <c r="E1573" s="148"/>
+      <c r="C1573" s="151"/>
+      <c r="D1573" s="152"/>
+      <c r="E1573" s="152"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -17463,9 +17489,9 @@
         <v>116</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="147"/>
-      <c r="D1590" s="148"/>
-      <c r="E1590" s="148"/>
+      <c r="C1590" s="151"/>
+      <c r="D1590" s="152"/>
+      <c r="E1590" s="152"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -17616,9 +17642,9 @@
         <v>117</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="147"/>
-      <c r="D1607" s="148"/>
-      <c r="E1607" s="148"/>
+      <c r="C1607" s="151"/>
+      <c r="D1607" s="152"/>
+      <c r="E1607" s="152"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -17769,9 +17795,9 @@
         <v>118</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="147"/>
-      <c r="D1624" s="148"/>
-      <c r="E1624" s="148"/>
+      <c r="C1624" s="151"/>
+      <c r="D1624" s="152"/>
+      <c r="E1624" s="152"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -17922,18 +17948,18 @@
         <v>119</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="153"/>
-      <c r="D1641" s="154"/>
-      <c r="E1641" s="154"/>
+      <c r="C1641" s="165"/>
+      <c r="D1641" s="166"/>
+      <c r="E1641" s="166"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>120</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="147"/>
-      <c r="D1642" s="148"/>
-      <c r="E1642" s="148"/>
+      <c r="C1642" s="151"/>
+      <c r="D1642" s="152"/>
+      <c r="E1642" s="152"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -18084,9 +18110,9 @@
         <v>121</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="149"/>
-      <c r="D1659" s="150"/>
-      <c r="E1659" s="150"/>
+      <c r="C1659" s="153"/>
+      <c r="D1659" s="154"/>
+      <c r="E1659" s="154"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -18237,9 +18263,9 @@
         <v>122</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="147"/>
-      <c r="D1676" s="148"/>
-      <c r="E1676" s="148"/>
+      <c r="C1676" s="151"/>
+      <c r="D1676" s="152"/>
+      <c r="E1676" s="152"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -18390,9 +18416,9 @@
         <v>123</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="147"/>
-      <c r="D1693" s="148"/>
-      <c r="E1693" s="148"/>
+      <c r="C1693" s="151"/>
+      <c r="D1693" s="152"/>
+      <c r="E1693" s="152"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -18543,9 +18569,9 @@
         <v>124</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="147"/>
-      <c r="D1710" s="148"/>
-      <c r="E1710" s="148"/>
+      <c r="C1710" s="151"/>
+      <c r="D1710" s="152"/>
+      <c r="E1710" s="152"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -18696,9 +18722,9 @@
         <v>125</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="147"/>
-      <c r="D1727" s="148"/>
-      <c r="E1727" s="148"/>
+      <c r="C1727" s="151"/>
+      <c r="D1727" s="152"/>
+      <c r="E1727" s="152"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -18849,9 +18875,9 @@
         <v>126</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="147"/>
-      <c r="D1744" s="148"/>
-      <c r="E1744" s="148"/>
+      <c r="C1744" s="151"/>
+      <c r="D1744" s="152"/>
+      <c r="E1744" s="152"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -19002,9 +19028,9 @@
         <v>127</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="147"/>
-      <c r="D1761" s="148"/>
-      <c r="E1761" s="148"/>
+      <c r="C1761" s="151"/>
+      <c r="D1761" s="152"/>
+      <c r="E1761" s="152"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -19155,9 +19181,9 @@
         <v>128</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="147"/>
-      <c r="D1778" s="148"/>
-      <c r="E1778" s="148"/>
+      <c r="C1778" s="151"/>
+      <c r="D1778" s="152"/>
+      <c r="E1778" s="152"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -19308,9 +19334,9 @@
         <v>129</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="147"/>
-      <c r="D1795" s="148"/>
-      <c r="E1795" s="148"/>
+      <c r="C1795" s="151"/>
+      <c r="D1795" s="152"/>
+      <c r="E1795" s="152"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -19461,9 +19487,9 @@
         <v>130</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="147"/>
-      <c r="D1812" s="148"/>
-      <c r="E1812" s="148"/>
+      <c r="C1812" s="151"/>
+      <c r="D1812" s="152"/>
+      <c r="E1812" s="152"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -19614,9 +19640,9 @@
         <v>95</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="147"/>
-      <c r="D1829" s="148"/>
-      <c r="E1829" s="148"/>
+      <c r="C1829" s="151"/>
+      <c r="D1829" s="152"/>
+      <c r="E1829" s="152"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -19767,9 +19793,9 @@
         <v>131</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="147"/>
-      <c r="D1846" s="148"/>
-      <c r="E1846" s="148"/>
+      <c r="C1846" s="151"/>
+      <c r="D1846" s="152"/>
+      <c r="E1846" s="152"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -19920,9 +19946,9 @@
         <v>132</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="147"/>
-      <c r="D1863" s="148"/>
-      <c r="E1863" s="148"/>
+      <c r="C1863" s="151"/>
+      <c r="D1863" s="152"/>
+      <c r="E1863" s="152"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -20073,9 +20099,9 @@
         <v>133</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="147"/>
-      <c r="D1880" s="148"/>
-      <c r="E1880" s="148"/>
+      <c r="C1880" s="151"/>
+      <c r="D1880" s="152"/>
+      <c r="E1880" s="152"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -20226,9 +20252,9 @@
         <v>134</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="147"/>
-      <c r="D1897" s="148"/>
-      <c r="E1897" s="148"/>
+      <c r="C1897" s="151"/>
+      <c r="D1897" s="152"/>
+      <c r="E1897" s="152"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -20379,18 +20405,18 @@
         <v>135</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="151"/>
-      <c r="D1914" s="152"/>
-      <c r="E1914" s="152"/>
+      <c r="C1914" s="167"/>
+      <c r="D1914" s="168"/>
+      <c r="E1914" s="168"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>136</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="147"/>
-      <c r="D1915" s="148"/>
-      <c r="E1915" s="148"/>
+      <c r="C1915" s="151"/>
+      <c r="D1915" s="152"/>
+      <c r="E1915" s="152"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -20541,9 +20567,9 @@
         <v>137</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="149"/>
-      <c r="D1932" s="150"/>
-      <c r="E1932" s="150"/>
+      <c r="C1932" s="153"/>
+      <c r="D1932" s="154"/>
+      <c r="E1932" s="154"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -20694,9 +20720,9 @@
         <v>138</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="147"/>
-      <c r="D1949" s="148"/>
-      <c r="E1949" s="148"/>
+      <c r="C1949" s="151"/>
+      <c r="D1949" s="152"/>
+      <c r="E1949" s="152"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -20847,9 +20873,9 @@
         <v>139</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="147"/>
-      <c r="D1966" s="148"/>
-      <c r="E1966" s="148"/>
+      <c r="C1966" s="151"/>
+      <c r="D1966" s="152"/>
+      <c r="E1966" s="152"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -21000,9 +21026,9 @@
         <v>140</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="147"/>
-      <c r="D1983" s="148"/>
-      <c r="E1983" s="148"/>
+      <c r="C1983" s="151"/>
+      <c r="D1983" s="152"/>
+      <c r="E1983" s="152"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -21153,9 +21179,9 @@
         <v>141</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="147"/>
-      <c r="D2000" s="148"/>
-      <c r="E2000" s="148"/>
+      <c r="C2000" s="151"/>
+      <c r="D2000" s="152"/>
+      <c r="E2000" s="152"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -21306,9 +21332,9 @@
         <v>142</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="147"/>
-      <c r="D2017" s="148"/>
-      <c r="E2017" s="148"/>
+      <c r="C2017" s="151"/>
+      <c r="D2017" s="152"/>
+      <c r="E2017" s="152"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -21459,9 +21485,9 @@
         <v>143</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="147"/>
-      <c r="D2034" s="148"/>
-      <c r="E2034" s="148"/>
+      <c r="C2034" s="151"/>
+      <c r="D2034" s="152"/>
+      <c r="E2034" s="152"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -21612,9 +21638,9 @@
         <v>144</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="147"/>
-      <c r="D2051" s="148"/>
-      <c r="E2051" s="148"/>
+      <c r="C2051" s="151"/>
+      <c r="D2051" s="152"/>
+      <c r="E2051" s="152"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -21765,9 +21791,9 @@
         <v>145</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="147"/>
-      <c r="D2068" s="148"/>
-      <c r="E2068" s="148"/>
+      <c r="C2068" s="151"/>
+      <c r="D2068" s="152"/>
+      <c r="E2068" s="152"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -21918,9 +21944,9 @@
         <v>146</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="147"/>
-      <c r="D2085" s="148"/>
-      <c r="E2085" s="148"/>
+      <c r="C2085" s="151"/>
+      <c r="D2085" s="152"/>
+      <c r="E2085" s="152"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -22071,9 +22097,9 @@
         <v>147</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="147"/>
-      <c r="D2102" s="148"/>
-      <c r="E2102" s="148"/>
+      <c r="C2102" s="151"/>
+      <c r="D2102" s="152"/>
+      <c r="E2102" s="152"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -22224,9 +22250,9 @@
         <v>96</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="147"/>
-      <c r="D2119" s="148"/>
-      <c r="E2119" s="148"/>
+      <c r="C2119" s="151"/>
+      <c r="D2119" s="152"/>
+      <c r="E2119" s="152"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -22377,9 +22403,9 @@
         <v>148</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="147"/>
-      <c r="D2136" s="148"/>
-      <c r="E2136" s="148"/>
+      <c r="C2136" s="151"/>
+      <c r="D2136" s="152"/>
+      <c r="E2136" s="152"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -22530,9 +22556,9 @@
         <v>149</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="147"/>
-      <c r="D2153" s="148"/>
-      <c r="E2153" s="148"/>
+      <c r="C2153" s="151"/>
+      <c r="D2153" s="152"/>
+      <c r="E2153" s="152"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -22683,9 +22709,9 @@
         <v>150</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="147"/>
-      <c r="D2170" s="148"/>
-      <c r="E2170" s="148"/>
+      <c r="C2170" s="151"/>
+      <c r="D2170" s="152"/>
+      <c r="E2170" s="152"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -22833,26 +22859,111 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
     <mergeCell ref="C430:E430"/>
@@ -22865,113 +22976,28 @@
     <mergeCell ref="C345:E345"/>
     <mergeCell ref="C362:E362"/>
     <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -22996,51 +23022,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="174" t="s">
+      <c r="A1" s="175" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="174"/>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
-      <c r="G1" s="174"/>
-      <c r="H1" s="174"/>
-      <c r="I1" s="174"/>
-      <c r="J1" s="174"/>
-      <c r="K1" s="174"/>
-      <c r="L1" s="174"/>
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="175"/>
+      <c r="H1" s="175"/>
+      <c r="I1" s="175"/>
+      <c r="J1" s="175"/>
+      <c r="K1" s="175"/>
+      <c r="L1" s="175"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="172" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="172"/>
-      <c r="C2" s="172"/>
-      <c r="D2" s="172"/>
-      <c r="E2" s="172"/>
-      <c r="F2" s="172"/>
-      <c r="G2" s="172"/>
-      <c r="H2" s="172"/>
-      <c r="I2" s="172"/>
-      <c r="J2" s="172"/>
-      <c r="K2" s="172"/>
-      <c r="L2" s="173"/>
+      <c r="B2" s="173"/>
+      <c r="C2" s="173"/>
+      <c r="D2" s="173"/>
+      <c r="E2" s="173"/>
+      <c r="F2" s="173"/>
+      <c r="G2" s="173"/>
+      <c r="H2" s="173"/>
+      <c r="I2" s="173"/>
+      <c r="J2" s="173"/>
+      <c r="K2" s="173"/>
+      <c r="L2" s="174"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="169" t="s">
         <v>157</v>
       </c>
-      <c r="B3" s="169"/>
-      <c r="C3" s="169"/>
-      <c r="D3" s="169"/>
-      <c r="E3" s="169"/>
-      <c r="F3" s="169"/>
-      <c r="G3" s="169"/>
-      <c r="H3" s="169"/>
-      <c r="I3" s="169"/>
-      <c r="J3" s="169"/>
-      <c r="K3" s="170"/>
+      <c r="B3" s="170"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="170"/>
+      <c r="H3" s="170"/>
+      <c r="I3" s="170"/>
+      <c r="J3" s="170"/>
+      <c r="K3" s="171"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1">
       <c r="A4" s="28" t="s">
@@ -23257,19 +23283,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A20" s="168" t="s">
+      <c r="A20" s="169" t="s">
         <v>165</v>
       </c>
-      <c r="B20" s="169"/>
-      <c r="C20" s="169"/>
-      <c r="D20" s="169"/>
-      <c r="E20" s="169"/>
-      <c r="F20" s="169"/>
-      <c r="G20" s="169"/>
-      <c r="H20" s="169"/>
-      <c r="I20" s="169"/>
-      <c r="J20" s="169"/>
-      <c r="K20" s="170"/>
+      <c r="B20" s="170"/>
+      <c r="C20" s="170"/>
+      <c r="D20" s="170"/>
+      <c r="E20" s="170"/>
+      <c r="F20" s="170"/>
+      <c r="G20" s="170"/>
+      <c r="H20" s="170"/>
+      <c r="I20" s="170"/>
+      <c r="J20" s="170"/>
+      <c r="K20" s="171"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="28" t="s">
@@ -23486,19 +23512,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A37" s="168" t="s">
+      <c r="A37" s="169" t="s">
         <v>166</v>
       </c>
-      <c r="B37" s="169"/>
-      <c r="C37" s="169"/>
-      <c r="D37" s="169"/>
-      <c r="E37" s="169"/>
-      <c r="F37" s="169"/>
-      <c r="G37" s="169"/>
-      <c r="H37" s="169"/>
-      <c r="I37" s="169"/>
-      <c r="J37" s="169"/>
-      <c r="K37" s="170"/>
+      <c r="B37" s="170"/>
+      <c r="C37" s="170"/>
+      <c r="D37" s="170"/>
+      <c r="E37" s="170"/>
+      <c r="F37" s="170"/>
+      <c r="G37" s="170"/>
+      <c r="H37" s="170"/>
+      <c r="I37" s="170"/>
+      <c r="J37" s="170"/>
+      <c r="K37" s="171"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="28" t="s">
@@ -23722,7 +23748,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -23756,28 +23782,28 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="175"/>
+      <c r="A3" s="176"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="176"/>
+      <c r="A4" s="177"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="176"/>
+      <c r="A5" s="177"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="176"/>
+      <c r="A6" s="177"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="176"/>
+      <c r="A7" s="177"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="176"/>
+      <c r="A8" s="177"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="176"/>
+      <c r="A9" s="177"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1">
-      <c r="A10" s="177"/>
+      <c r="A10" s="178"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1">
       <c r="A11" s="22" t="s">
@@ -23933,7 +23959,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -23960,10 +23986,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="178" t="s">
+      <c r="B1" s="179" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="179"/>
+      <c r="C1" s="180"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -23974,7 +24000,7 @@
       <c r="E2" s="109"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="180" t="s">
+      <c r="A3" s="181" t="s">
         <v>201</v>
       </c>
       <c r="B3" s="117" t="s">
@@ -23988,7 +24014,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="181"/>
+      <c r="A4" s="182"/>
       <c r="B4" s="114" t="s">
         <v>158</v>
       </c>
@@ -24000,7 +24026,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="181"/>
+      <c r="A5" s="182"/>
       <c r="B5" s="114" t="s">
         <v>159</v>
       </c>
@@ -24009,7 +24035,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="181"/>
+      <c r="A6" s="182"/>
       <c r="B6" s="125" t="s">
         <v>203</v>
       </c>
@@ -24021,7 +24047,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="181"/>
+      <c r="A7" s="182"/>
       <c r="B7" s="114" t="s">
         <v>169</v>
       </c>
@@ -24033,7 +24059,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="181"/>
+      <c r="A8" s="182"/>
       <c r="B8" s="114" t="s">
         <v>170</v>
       </c>
@@ -24042,7 +24068,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="182"/>
+      <c r="A9" s="183"/>
       <c r="B9" s="122" t="s">
         <v>160</v>
       </c>
@@ -24057,7 +24083,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="180" t="s">
+      <c r="A11" s="181" t="s">
         <v>202</v>
       </c>
       <c r="B11" s="117" t="s">
@@ -24071,7 +24097,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="181"/>
+      <c r="A12" s="182"/>
       <c r="B12" s="114" t="s">
         <v>158</v>
       </c>
@@ -24083,7 +24109,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="181"/>
+      <c r="A13" s="182"/>
       <c r="B13" s="114" t="s">
         <v>159</v>
       </c>
@@ -24092,7 +24118,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="181"/>
+      <c r="A14" s="182"/>
       <c r="B14" s="125" t="s">
         <v>203</v>
       </c>
@@ -24104,7 +24130,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="181"/>
+      <c r="A15" s="182"/>
       <c r="B15" s="114" t="s">
         <v>169</v>
       </c>
@@ -24116,7 +24142,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="181"/>
+      <c r="A16" s="182"/>
       <c r="B16" s="114" t="s">
         <v>170</v>
       </c>
@@ -24125,7 +24151,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="182"/>
+      <c r="A17" s="183"/>
       <c r="B17" s="122" t="s">
         <v>160</v>
       </c>
@@ -24140,7 +24166,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="180" t="s">
+      <c r="A19" s="181" t="s">
         <v>202</v>
       </c>
       <c r="B19" s="117" t="s">
@@ -24149,7 +24175,7 @@
       <c r="C19" s="116"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="181"/>
+      <c r="A20" s="182"/>
       <c r="B20" s="114" t="s">
         <v>158</v>
       </c>
@@ -24159,14 +24185,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="181"/>
+      <c r="A21" s="182"/>
       <c r="B21" s="114" t="s">
         <v>159</v>
       </c>
       <c r="C21" s="119"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="181"/>
+      <c r="A22" s="182"/>
       <c r="B22" s="125" t="s">
         <v>203</v>
       </c>
@@ -24176,7 +24202,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="181"/>
+      <c r="A23" s="182"/>
       <c r="B23" s="114" t="s">
         <v>169</v>
       </c>
@@ -24186,14 +24212,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="181"/>
+      <c r="A24" s="182"/>
       <c r="B24" s="114" t="s">
         <v>170</v>
       </c>
       <c r="C24" s="118"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="182"/>
+      <c r="A25" s="183"/>
       <c r="B25" s="122" t="s">
         <v>160</v>
       </c>
@@ -24206,7 +24232,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -24228,163 +24254,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="192" t="s">
+      <c r="A1" s="194" t="s">
         <v>183</v>
       </c>
-      <c r="B1" s="193"/>
+      <c r="B1" s="195"/>
       <c r="C1" s="108"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="189" t="s">
+      <c r="A2" s="200" t="s">
         <v>182</v>
       </c>
-      <c r="B2" s="190"/>
+      <c r="B2" s="201"/>
       <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="191" t="s">
+      <c r="A3" s="202" t="s">
         <v>184</v>
       </c>
-      <c r="B3" s="190"/>
+      <c r="B3" s="201"/>
       <c r="C3" s="110"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="196"/>
-      <c r="B4" s="197"/>
+      <c r="A4" s="198"/>
+      <c r="B4" s="199"/>
       <c r="C4" s="110"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="194" t="s">
+      <c r="A5" s="196" t="s">
         <v>193</v>
       </c>
-      <c r="B5" s="195"/>
+      <c r="B5" s="197"/>
       <c r="C5" s="110"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="200" t="s">
+      <c r="A7" s="188" t="s">
         <v>185</v>
       </c>
-      <c r="B7" s="201"/>
+      <c r="B7" s="189"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="110"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="198" t="s">
+      <c r="A9" s="190" t="s">
         <v>186</v>
       </c>
-      <c r="B9" s="199"/>
+      <c r="B9" s="191"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="185"/>
-      <c r="B10" s="186"/>
+      <c r="A10" s="192"/>
+      <c r="B10" s="193"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="187" t="s">
+      <c r="A11" s="184" t="s">
         <v>187</v>
       </c>
-      <c r="B11" s="188"/>
+      <c r="B11" s="185"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="187" t="s">
+      <c r="A12" s="184" t="s">
         <v>188</v>
       </c>
-      <c r="B12" s="188"/>
+      <c r="B12" s="185"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="187" t="s">
+      <c r="A13" s="184" t="s">
         <v>189</v>
       </c>
-      <c r="B13" s="188"/>
+      <c r="B13" s="185"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="187" t="s">
+      <c r="A14" s="184" t="s">
         <v>190</v>
       </c>
-      <c r="B14" s="188"/>
+      <c r="B14" s="185"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="187" t="s">
+      <c r="A15" s="184" t="s">
         <v>191</v>
       </c>
-      <c r="B15" s="188"/>
+      <c r="B15" s="185"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="187" t="s">
+      <c r="A16" s="184" t="s">
         <v>192</v>
       </c>
-      <c r="B16" s="188"/>
+      <c r="B16" s="185"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="183" t="s">
+      <c r="A17" s="186" t="s">
         <v>194</v>
       </c>
-      <c r="B17" s="184"/>
+      <c r="B17" s="187"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="200" t="s">
+      <c r="A19" s="188" t="s">
         <v>196</v>
       </c>
-      <c r="B19" s="201"/>
+      <c r="B19" s="189"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="110"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="198" t="s">
+      <c r="A21" s="190" t="s">
         <v>197</v>
       </c>
-      <c r="B21" s="199"/>
+      <c r="B21" s="191"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="185"/>
-      <c r="B22" s="186"/>
+      <c r="A22" s="192"/>
+      <c r="B22" s="193"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="187" t="s">
+      <c r="A23" s="184" t="s">
         <v>198</v>
       </c>
-      <c r="B23" s="188"/>
+      <c r="B23" s="185"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="187"/>
-      <c r="B24" s="188"/>
+      <c r="A24" s="184"/>
+      <c r="B24" s="185"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="187" t="s">
+      <c r="A25" s="184" t="s">
         <v>199</v>
       </c>
-      <c r="B25" s="188"/>
+      <c r="B25" s="185"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="187" t="s">
+      <c r="A26" s="184" t="s">
         <v>200</v>
       </c>
-      <c r="B26" s="188"/>
+      <c r="B26" s="185"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="183"/>
-      <c r="B27" s="184"/>
+      <c r="A27" s="186"/>
+      <c r="B27" s="187"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -24395,6 +24408,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>